<commit_message>
feat: update sales resources
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-sales-template-2024-25.xlsx
+++ b/public/files/bulk-upload-sales-template-2024-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 Annual log changes/2024-25/03 Materials for providers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{CD602663-1CCE-42E7-A578-0D2CBA61949F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24C1F701-145D-49F7-B68D-47664BB64896}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7D1A7-CEC5-402E-A9C5-E5E0C01F6637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24-25 Sales template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="271">
   <si>
     <t>Section</t>
   </si>
@@ -823,12 +823,6 @@
 Yes, if the purchase was a staircasing transaction (if field 86 = 1)</t>
   </si>
   <si>
-    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or if a mortgage was not used (if field 103 = 2)</t>
-  </si>
-  <si>
-    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3), if a mortgage was not used (if field 103 = 2) or if 'Other' is not selected for mortgage lender name (if field 105 is not 40)</t>
-  </si>
-  <si>
     <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or the type of shared ownership sale is not Social Homebuy (if field 9 is not 18)</t>
   </si>
   <si>
@@ -865,6 +859,15 @@
   </si>
   <si>
     <t>Field number</t>
+  </si>
+  <si>
+    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or if a mortgage was not used (if field 103 = 2 or 3)</t>
+  </si>
+  <si>
+    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3), if a mortgage was not used (if field 103 = 2 or 3) or if 'Other' is not selected for mortgage lender name (if field 105 is not 40)</t>
+  </si>
+  <si>
+    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or if mortgage information is unknown (field 103 = 3)</t>
   </si>
 </sst>
 </file>
@@ -1428,66 +1431,167 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1497,136 +1601,35 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1851,7 +1854,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1883,155 +1886,155 @@
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="81" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="81"/>
-      <c r="V1" s="81"/>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="81"/>
-      <c r="Z1" s="81"/>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="81"/>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="56" t="s">
+      <c r="U1" s="106"/>
+      <c r="V1" s="106"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="106"/>
+      <c r="Y1" s="106"/>
+      <c r="Z1" s="106"/>
+      <c r="AA1" s="106"/>
+      <c r="AB1" s="106"/>
+      <c r="AC1" s="106"/>
+      <c r="AD1" s="106"/>
+      <c r="AE1" s="106"/>
+      <c r="AF1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="56"/>
-      <c r="AL1" s="56"/>
-      <c r="AM1" s="56"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="56"/>
-      <c r="AQ1" s="56"/>
-      <c r="AR1" s="56"/>
-      <c r="AS1" s="56"/>
-      <c r="AT1" s="56"/>
-      <c r="AU1" s="56"/>
-      <c r="AV1" s="56"/>
-      <c r="AW1" s="56"/>
-      <c r="AX1" s="56"/>
-      <c r="AY1" s="56"/>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="56"/>
-      <c r="BB1" s="56"/>
-      <c r="BC1" s="56"/>
-      <c r="BD1" s="56"/>
-      <c r="BE1" s="56"/>
-      <c r="BF1" s="56"/>
-      <c r="BG1" s="56"/>
-      <c r="BH1" s="56"/>
-      <c r="BI1" s="56"/>
-      <c r="BJ1" s="82" t="s">
+      <c r="AG1" s="107"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="107"/>
+      <c r="AJ1" s="107"/>
+      <c r="AK1" s="107"/>
+      <c r="AL1" s="107"/>
+      <c r="AM1" s="107"/>
+      <c r="AN1" s="107"/>
+      <c r="AO1" s="107"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="107"/>
+      <c r="AR1" s="107"/>
+      <c r="AS1" s="107"/>
+      <c r="AT1" s="107"/>
+      <c r="AU1" s="107"/>
+      <c r="AV1" s="107"/>
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="107"/>
+      <c r="AZ1" s="107"/>
+      <c r="BA1" s="107"/>
+      <c r="BB1" s="107"/>
+      <c r="BC1" s="107"/>
+      <c r="BD1" s="107"/>
+      <c r="BE1" s="107"/>
+      <c r="BF1" s="107"/>
+      <c r="BG1" s="107"/>
+      <c r="BH1" s="107"/>
+      <c r="BI1" s="107"/>
+      <c r="BJ1" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="BK1" s="82"/>
-      <c r="BL1" s="82"/>
-      <c r="BM1" s="82"/>
-      <c r="BN1" s="82"/>
-      <c r="BO1" s="82"/>
-      <c r="BP1" s="82"/>
-      <c r="BQ1" s="82"/>
-      <c r="BR1" s="82"/>
-      <c r="BS1" s="82"/>
-      <c r="BT1" s="82"/>
-      <c r="BU1" s="55" t="s">
+      <c r="BK1" s="108"/>
+      <c r="BL1" s="108"/>
+      <c r="BM1" s="108"/>
+      <c r="BN1" s="108"/>
+      <c r="BO1" s="108"/>
+      <c r="BP1" s="108"/>
+      <c r="BQ1" s="108"/>
+      <c r="BR1" s="108"/>
+      <c r="BS1" s="108"/>
+      <c r="BT1" s="108"/>
+      <c r="BU1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="BV1" s="55"/>
-      <c r="BW1" s="55"/>
-      <c r="BX1" s="55"/>
-      <c r="BY1" s="55"/>
-      <c r="BZ1" s="83" t="s">
+      <c r="BV1" s="109"/>
+      <c r="BW1" s="109"/>
+      <c r="BX1" s="109"/>
+      <c r="BY1" s="109"/>
+      <c r="BZ1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="CA1" s="83"/>
-      <c r="CB1" s="83"/>
-      <c r="CC1" s="83"/>
-      <c r="CD1" s="83"/>
-      <c r="CE1" s="83"/>
-      <c r="CF1" s="83"/>
-      <c r="CG1" s="83"/>
-      <c r="CH1" s="54" t="s">
+      <c r="CA1" s="98"/>
+      <c r="CB1" s="98"/>
+      <c r="CC1" s="98"/>
+      <c r="CD1" s="98"/>
+      <c r="CE1" s="98"/>
+      <c r="CF1" s="98"/>
+      <c r="CG1" s="98"/>
+      <c r="CH1" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="CI1" s="54"/>
-      <c r="CJ1" s="54"/>
-      <c r="CK1" s="54"/>
-      <c r="CL1" s="54"/>
-      <c r="CM1" s="54"/>
-      <c r="CN1" s="54"/>
-      <c r="CO1" s="54"/>
-      <c r="CP1" s="54"/>
-      <c r="CQ1" s="54"/>
-      <c r="CR1" s="54"/>
-      <c r="CS1" s="54"/>
-      <c r="CT1" s="54"/>
-      <c r="CU1" s="54"/>
-      <c r="CV1" s="54"/>
-      <c r="CW1" s="54"/>
-      <c r="CX1" s="54"/>
-      <c r="CY1" s="54"/>
-      <c r="CZ1" s="54"/>
-      <c r="DA1" s="54"/>
-      <c r="DB1" s="54"/>
-      <c r="DC1" s="54"/>
-      <c r="DD1" s="54"/>
-      <c r="DE1" s="54"/>
-      <c r="DF1" s="54"/>
-      <c r="DG1" s="54"/>
-      <c r="DH1" s="54"/>
-      <c r="DI1" s="54"/>
-      <c r="DJ1" s="55" t="s">
+      <c r="CI1" s="122"/>
+      <c r="CJ1" s="122"/>
+      <c r="CK1" s="122"/>
+      <c r="CL1" s="122"/>
+      <c r="CM1" s="122"/>
+      <c r="CN1" s="122"/>
+      <c r="CO1" s="122"/>
+      <c r="CP1" s="122"/>
+      <c r="CQ1" s="122"/>
+      <c r="CR1" s="122"/>
+      <c r="CS1" s="122"/>
+      <c r="CT1" s="122"/>
+      <c r="CU1" s="122"/>
+      <c r="CV1" s="122"/>
+      <c r="CW1" s="122"/>
+      <c r="CX1" s="122"/>
+      <c r="CY1" s="122"/>
+      <c r="CZ1" s="122"/>
+      <c r="DA1" s="122"/>
+      <c r="DB1" s="122"/>
+      <c r="DC1" s="122"/>
+      <c r="DD1" s="122"/>
+      <c r="DE1" s="122"/>
+      <c r="DF1" s="122"/>
+      <c r="DG1" s="122"/>
+      <c r="DH1" s="122"/>
+      <c r="DI1" s="122"/>
+      <c r="DJ1" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="DK1" s="55"/>
-      <c r="DL1" s="55"/>
-      <c r="DM1" s="55"/>
-      <c r="DN1" s="55"/>
-      <c r="DO1" s="55"/>
-      <c r="DP1" s="55"/>
-      <c r="DQ1" s="55"/>
-      <c r="DR1" s="55"/>
-      <c r="DS1" s="55"/>
-      <c r="DT1" s="55"/>
-      <c r="DU1" s="55"/>
-      <c r="DV1" s="56" t="s">
+      <c r="DK1" s="109"/>
+      <c r="DL1" s="109"/>
+      <c r="DM1" s="109"/>
+      <c r="DN1" s="109"/>
+      <c r="DO1" s="109"/>
+      <c r="DP1" s="109"/>
+      <c r="DQ1" s="109"/>
+      <c r="DR1" s="109"/>
+      <c r="DS1" s="109"/>
+      <c r="DT1" s="109"/>
+      <c r="DU1" s="109"/>
+      <c r="DV1" s="107" t="s">
         <v>222</v>
       </c>
-      <c r="DW1" s="56"/>
-      <c r="DX1" s="56"/>
-      <c r="DY1" s="56"/>
-      <c r="DZ1" s="56"/>
-      <c r="EA1" s="56"/>
-      <c r="EB1" s="56"/>
+      <c r="DW1" s="107"/>
+      <c r="DX1" s="107"/>
+      <c r="DY1" s="107"/>
+      <c r="DZ1" s="107"/>
+      <c r="EA1" s="107"/>
+      <c r="EB1" s="107"/>
     </row>
     <row r="2" spans="1:132" ht="115" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2041,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -2431,271 +2434,271 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:132" s="121" customFormat="1" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:132" s="68" customFormat="1" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="70" t="s">
         <v>197</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="K3" s="103" t="s">
+      <c r="K3" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="M3" s="104"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103" t="s">
+      <c r="M3" s="57"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103" t="s">
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="S3" s="105" t="s">
-        <v>268</v>
-      </c>
-      <c r="T3" s="106" t="s">
+      <c r="S3" s="58" t="s">
+        <v>266</v>
+      </c>
+      <c r="T3" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="107" t="s">
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="101"/>
-      <c r="AA3" s="101"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
       <c r="AB3" s="27" t="s">
         <v>211</v>
       </c>
       <c r="AC3" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="AD3" s="101"/>
-      <c r="AE3" s="103" t="s">
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="AF3" s="101" t="s">
+      <c r="AF3" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="AG3" s="101" t="s">
+      <c r="AG3" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="AH3" s="101"/>
-      <c r="AI3" s="108" t="s">
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="AJ3" s="106" t="s">
+      <c r="AJ3" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="AK3" s="109"/>
-      <c r="AL3" s="109"/>
-      <c r="AM3" s="109"/>
-      <c r="AN3" s="106" t="s">
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="62"/>
+      <c r="AM3" s="62"/>
+      <c r="AN3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="AO3" s="106"/>
-      <c r="AP3" s="108" t="s">
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="AQ3" s="106"/>
-      <c r="AR3" s="106"/>
-      <c r="AS3" s="106" t="s">
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="59"/>
+      <c r="AS3" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="AT3" s="106"/>
-      <c r="AU3" s="106"/>
-      <c r="AV3" s="106" t="s">
+      <c r="AT3" s="59"/>
+      <c r="AU3" s="59"/>
+      <c r="AV3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="AW3" s="106"/>
-      <c r="AX3" s="106"/>
-      <c r="AY3" s="106"/>
-      <c r="AZ3" s="106" t="s">
+      <c r="AW3" s="59"/>
+      <c r="AX3" s="59"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="BA3" s="106"/>
-      <c r="BB3" s="106"/>
-      <c r="BC3" s="106"/>
-      <c r="BD3" s="106" t="s">
+      <c r="BA3" s="59"/>
+      <c r="BB3" s="59"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="BE3" s="106"/>
-      <c r="BF3" s="106"/>
-      <c r="BG3" s="106"/>
-      <c r="BH3" s="106" t="s">
+      <c r="BE3" s="59"/>
+      <c r="BF3" s="59"/>
+      <c r="BG3" s="59"/>
+      <c r="BH3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="BI3" s="106"/>
-      <c r="BJ3" s="101"/>
-      <c r="BK3" s="110" t="s">
+      <c r="BI3" s="59"/>
+      <c r="BJ3" s="54"/>
+      <c r="BK3" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="BL3" s="111"/>
-      <c r="BM3" s="111"/>
-      <c r="BN3" s="112"/>
-      <c r="BO3" s="113"/>
-      <c r="BP3" s="101"/>
-      <c r="BQ3" s="101"/>
-      <c r="BR3" s="114"/>
-      <c r="BS3" s="106"/>
-      <c r="BT3" s="106"/>
-      <c r="BU3" s="115" t="s">
+      <c r="BL3" s="102"/>
+      <c r="BM3" s="102"/>
+      <c r="BN3" s="103"/>
+      <c r="BO3" s="63"/>
+      <c r="BP3" s="54"/>
+      <c r="BQ3" s="54"/>
+      <c r="BR3" s="64"/>
+      <c r="BS3" s="59"/>
+      <c r="BT3" s="59"/>
+      <c r="BU3" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="BV3" s="115"/>
-      <c r="BW3" s="115" t="s">
+      <c r="BV3" s="65"/>
+      <c r="BW3" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="BX3" s="106" t="s">
+      <c r="BX3" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="BY3" s="106" t="s">
+      <c r="BY3" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="BZ3" s="106" t="s">
+      <c r="BZ3" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="CA3" s="106"/>
-      <c r="CB3" s="106" t="s">
+      <c r="CA3" s="59"/>
+      <c r="CB3" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="CC3" s="106"/>
-      <c r="CD3" s="106"/>
-      <c r="CE3" s="106" t="s">
+      <c r="CC3" s="59"/>
+      <c r="CD3" s="59"/>
+      <c r="CE3" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="CF3" s="106"/>
-      <c r="CG3" s="106" t="s">
+      <c r="CF3" s="59"/>
+      <c r="CG3" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="CH3" s="116" t="s">
+      <c r="CH3" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="CI3" s="106" t="s">
+      <c r="CI3" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="CJ3" s="106"/>
-      <c r="CK3" s="106"/>
-      <c r="CL3" s="106"/>
-      <c r="CM3" s="106" t="s">
+      <c r="CJ3" s="59"/>
+      <c r="CK3" s="59"/>
+      <c r="CL3" s="59"/>
+      <c r="CM3" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="CN3" s="117" t="s">
+      <c r="CN3" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="CO3" s="118"/>
-      <c r="CP3" s="119"/>
-      <c r="CQ3" s="117" t="s">
+      <c r="CO3" s="91"/>
+      <c r="CP3" s="92"/>
+      <c r="CQ3" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="CR3" s="118"/>
-      <c r="CS3" s="119"/>
-      <c r="CT3" s="106" t="s">
+      <c r="CR3" s="91"/>
+      <c r="CS3" s="92"/>
+      <c r="CT3" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="CU3" s="106" t="s">
+      <c r="CU3" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="CV3" s="106"/>
-      <c r="CW3" s="106"/>
-      <c r="CX3" s="106" t="s">
+      <c r="CV3" s="59"/>
+      <c r="CW3" s="59"/>
+      <c r="CX3" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="CY3" s="107" t="s">
+      <c r="CY3" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="CZ3" s="122" t="s">
-        <v>267</v>
+      <c r="CZ3" s="69" t="s">
+        <v>265</v>
       </c>
       <c r="DA3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="DB3" s="106"/>
-      <c r="DC3" s="116"/>
-      <c r="DD3" s="116"/>
-      <c r="DE3" s="106" t="s">
+      <c r="DB3" s="59"/>
+      <c r="DC3" s="66"/>
+      <c r="DD3" s="66"/>
+      <c r="DE3" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="DF3" s="106" t="s">
+      <c r="DF3" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="DG3" s="106" t="s">
+      <c r="DG3" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="DH3" s="106" t="s">
+      <c r="DH3" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="DI3" s="106" t="s">
+      <c r="DI3" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="DJ3" s="116"/>
-      <c r="DK3" s="106" t="s">
+      <c r="DJ3" s="66"/>
+      <c r="DK3" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="DL3" s="106" t="s">
+      <c r="DL3" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="DM3" s="101" t="s">
+      <c r="DM3" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="DN3" s="101"/>
+      <c r="DN3" s="54"/>
       <c r="DO3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="DP3" s="101"/>
-      <c r="DQ3" s="120"/>
-      <c r="DR3" s="120"/>
-      <c r="DS3" s="101" t="s">
+      <c r="DP3" s="54"/>
+      <c r="DQ3" s="67"/>
+      <c r="DR3" s="67"/>
+      <c r="DS3" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="DT3" s="101" t="s">
+      <c r="DT3" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="DU3" s="101" t="s">
+      <c r="DU3" s="54" t="s">
         <v>144</v>
       </c>
       <c r="DV3" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="DW3" s="101"/>
+      <c r="DW3" s="54"/>
       <c r="DX3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="DY3" s="120"/>
-      <c r="DZ3" s="101" t="s">
+      <c r="DY3" s="67"/>
+      <c r="DZ3" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="EA3" s="101" t="s">
+      <c r="EA3" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="EB3" s="101" t="s">
+      <c r="EB3" s="54" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:132" s="51" customFormat="1" ht="125" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:132" s="51" customFormat="1" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>150</v>
       </c>
@@ -2735,11 +2738,11 @@
       <c r="M4" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="N4" s="93" t="s">
+      <c r="N4" s="72" t="s">
         <v>158</v>
       </c>
-      <c r="O4" s="98"/>
-      <c r="P4" s="94"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="81"/>
       <c r="Q4" s="31" t="s">
         <v>153</v>
       </c>
@@ -2761,19 +2764,19 @@
       <c r="W4" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="57" t="s">
+      <c r="X4" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="89" t="s">
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="AA4" s="91"/>
+      <c r="AA4" s="73"/>
       <c r="AB4" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AC4" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AD4" s="49" t="s">
         <v>210</v>
@@ -2791,7 +2794,7 @@
         <v>216</v>
       </c>
       <c r="AI4" s="29" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AJ4" s="7" t="s">
         <v>165</v>
@@ -2812,7 +2815,7 @@
         <v>216</v>
       </c>
       <c r="AP4" s="29" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AQ4" s="7" t="s">
         <v>168</v>
@@ -2878,20 +2881,20 @@
         <v>158</v>
       </c>
       <c r="BL4" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BM4" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="BN4" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="BO4" s="85" t="s">
+      <c r="BO4" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="BP4" s="86"/>
-      <c r="BQ4" s="86"/>
-      <c r="BR4" s="86"/>
+      <c r="BP4" s="94"/>
+      <c r="BQ4" s="94"/>
+      <c r="BR4" s="94"/>
       <c r="BS4" s="5" t="s">
         <v>153</v>
       </c>
@@ -2907,10 +2910,10 @@
       <c r="BW4" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="BX4" s="57" t="s">
+      <c r="BX4" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="BY4" s="69"/>
+      <c r="BY4" s="75"/>
       <c r="BZ4" s="5" t="s">
         <v>175</v>
       </c>
@@ -2929,20 +2932,20 @@
       <c r="CE4" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="CF4" s="57" t="s">
+      <c r="CF4" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="CG4" s="69"/>
+      <c r="CG4" s="75"/>
       <c r="CH4" s="6" t="s">
         <v>178</v>
       </c>
       <c r="CI4" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="CJ4" s="57" t="s">
+      <c r="CJ4" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="CK4" s="69"/>
+      <c r="CK4" s="75"/>
       <c r="CL4" s="5" t="s">
         <v>153</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>152</v>
       </c>
       <c r="CP4" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="CQ4" s="5" t="s">
         <v>151</v>
@@ -2965,7 +2968,7 @@
         <v>152</v>
       </c>
       <c r="CS4" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="CT4" s="5" t="s">
         <v>153</v>
@@ -3003,21 +3006,21 @@
       <c r="DE4" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="DF4" s="57" t="s">
+      <c r="DF4" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="DG4" s="69"/>
-      <c r="DH4" s="57" t="s">
+      <c r="DG4" s="75"/>
+      <c r="DH4" s="74" t="s">
         <v>184</v>
       </c>
-      <c r="DI4" s="69"/>
+      <c r="DI4" s="75"/>
       <c r="DJ4" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="DK4" s="57" t="s">
+      <c r="DK4" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="DL4" s="69"/>
+      <c r="DL4" s="75"/>
       <c r="DM4" s="5" t="s">
         <v>182</v>
       </c>
@@ -3080,11 +3083,11 @@
       <c r="D5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="H5" s="28" t="s">
         <v>188</v>
       </c>
@@ -3103,10 +3106,10 @@
       <c r="M5" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="N5" s="93" t="s">
+      <c r="N5" s="72" t="s">
         <v>227</v>
       </c>
-      <c r="O5" s="94"/>
+      <c r="O5" s="81"/>
       <c r="P5" s="31" t="s">
         <v>187</v>
       </c>
@@ -3119,11 +3122,11 @@
       <c r="S5" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="T5" s="89" t="s">
+      <c r="T5" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="U5" s="90"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="73"/>
       <c r="W5" s="42" t="s">
         <v>237</v>
       </c>
@@ -3139,24 +3142,24 @@
       <c r="AA5" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AB5" s="93" t="s">
+      <c r="AB5" s="72" t="s">
         <v>239</v>
       </c>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="57" t="s">
+      <c r="AC5" s="73"/>
+      <c r="AD5" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="57" t="s">
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="AG5" s="75"/>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="57" t="s">
+      <c r="AG5" s="97"/>
+      <c r="AH5" s="97"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="AK5" s="69"/>
+      <c r="AK5" s="75"/>
       <c r="AL5" s="40" t="s">
         <v>231</v>
       </c>
@@ -3166,10 +3169,10 @@
       <c r="AN5" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="AO5" s="57" t="s">
+      <c r="AO5" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="AP5" s="69"/>
+      <c r="AP5" s="75"/>
       <c r="AQ5" s="5" t="s">
         <v>235</v>
       </c>
@@ -3179,49 +3182,49 @@
       <c r="AS5" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="AT5" s="60" t="s">
+      <c r="AT5" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="AU5" s="61"/>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="62"/>
-      <c r="AX5" s="60" t="s">
+      <c r="AU5" s="123"/>
+      <c r="AV5" s="123"/>
+      <c r="AW5" s="124"/>
+      <c r="AX5" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="61"/>
-      <c r="BA5" s="62"/>
-      <c r="BB5" s="60" t="s">
+      <c r="AY5" s="123"/>
+      <c r="AZ5" s="123"/>
+      <c r="BA5" s="124"/>
+      <c r="BB5" s="114" t="s">
         <v>242</v>
       </c>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="61"/>
-      <c r="BE5" s="62"/>
-      <c r="BF5" s="60" t="s">
+      <c r="BC5" s="123"/>
+      <c r="BD5" s="123"/>
+      <c r="BE5" s="124"/>
+      <c r="BF5" s="114" t="s">
         <v>243</v>
       </c>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="61"/>
-      <c r="BI5" s="62"/>
+      <c r="BG5" s="123"/>
+      <c r="BH5" s="123"/>
+      <c r="BI5" s="124"/>
       <c r="BJ5" s="31" t="s">
         <v>187</v>
       </c>
       <c r="BK5" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="BL5" s="87" t="s">
+      <c r="BL5" s="95" t="s">
         <v>245</v>
       </c>
-      <c r="BM5" s="88"/>
+      <c r="BM5" s="96"/>
       <c r="BN5" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="BO5" s="89" t="s">
+      <c r="BO5" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="BP5" s="90"/>
-      <c r="BQ5" s="90"/>
-      <c r="BR5" s="91"/>
+      <c r="BP5" s="88"/>
+      <c r="BQ5" s="88"/>
+      <c r="BR5" s="73"/>
       <c r="BS5" s="14" t="s">
         <v>236</v>
       </c>
@@ -3234,11 +3237,11 @@
       <c r="BV5" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="BW5" s="57" t="s">
+      <c r="BW5" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="BX5" s="75"/>
-      <c r="BY5" s="75"/>
+      <c r="BX5" s="97"/>
+      <c r="BY5" s="97"/>
       <c r="BZ5" s="5" t="s">
         <v>187</v>
       </c>
@@ -3251,72 +3254,72 @@
       <c r="CC5" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="CD5" s="57" t="s">
+      <c r="CD5" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="CE5" s="75"/>
-      <c r="CF5" s="75"/>
+      <c r="CE5" s="97"/>
+      <c r="CF5" s="97"/>
       <c r="CG5" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="CH5" s="57" t="s">
+      <c r="CH5" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="CI5" s="75"/>
-      <c r="CJ5" s="57" t="s">
+      <c r="CI5" s="97"/>
+      <c r="CJ5" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="CK5" s="75"/>
-      <c r="CL5" s="69"/>
+      <c r="CK5" s="97"/>
+      <c r="CL5" s="75"/>
       <c r="CM5" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="CN5" s="57" t="s">
+      <c r="CN5" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="CO5" s="75"/>
-      <c r="CP5" s="75"/>
-      <c r="CQ5" s="75"/>
-      <c r="CR5" s="75"/>
-      <c r="CS5" s="75"/>
+      <c r="CO5" s="97"/>
+      <c r="CP5" s="97"/>
+      <c r="CQ5" s="97"/>
+      <c r="CR5" s="97"/>
+      <c r="CS5" s="97"/>
       <c r="CT5" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="CU5" s="76" t="s">
+      <c r="CU5" s="111" t="s">
         <v>255</v>
       </c>
-      <c r="CV5" s="77"/>
-      <c r="CW5" s="78"/>
-      <c r="CX5" s="57" t="s">
+      <c r="CV5" s="112"/>
+      <c r="CW5" s="113"/>
+      <c r="CX5" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="CY5" s="75"/>
-      <c r="CZ5" s="75"/>
-      <c r="DA5" s="57" t="s">
+      <c r="CY5" s="97"/>
+      <c r="CZ5" s="97"/>
+      <c r="DA5" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="DB5" s="75"/>
+      <c r="DC5" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="DD5" s="82" t="s">
+        <v>268</v>
+      </c>
+      <c r="DE5" s="75"/>
+      <c r="DF5" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG5" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="DB5" s="69"/>
-      <c r="DC5" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="DD5" s="66" t="s">
-        <v>256</v>
-      </c>
-      <c r="DE5" s="69"/>
-      <c r="DF5" s="10" t="s">
+      <c r="DH5" s="82" t="s">
         <v>225</v>
       </c>
-      <c r="DG5" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="DH5" s="66" t="s">
-        <v>225</v>
-      </c>
-      <c r="DI5" s="69"/>
-      <c r="DJ5" s="57" t="s">
+      <c r="DI5" s="75"/>
+      <c r="DJ5" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="DK5" s="69"/>
+      <c r="DK5" s="75"/>
       <c r="DL5" s="5" t="s">
         <v>228</v>
       </c>
@@ -3326,48 +3329,48 @@
       <c r="DN5" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="DO5" s="60" t="s">
+      <c r="DO5" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="DP5" s="75"/>
+      <c r="DQ5" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="DR5" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="DS5" s="75"/>
+      <c r="DT5" s="115" t="s">
+        <v>226</v>
+      </c>
+      <c r="DU5" s="75"/>
+      <c r="DV5" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="DW5" s="97"/>
+      <c r="DX5" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="DP5" s="69"/>
-      <c r="DQ5" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="DR5" s="60" t="s">
+      <c r="DY5" s="114" t="s">
         <v>259</v>
       </c>
-      <c r="DS5" s="69"/>
-      <c r="DT5" s="58" t="s">
-        <v>226</v>
-      </c>
-      <c r="DU5" s="69"/>
-      <c r="DV5" s="57" t="s">
+      <c r="DZ5" s="97"/>
+      <c r="EA5" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="DW5" s="75"/>
-      <c r="DX5" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="DY5" s="60" t="s">
-        <v>261</v>
-      </c>
-      <c r="DZ5" s="75"/>
-      <c r="EA5" s="57" t="s">
-        <v>227</v>
-      </c>
-      <c r="EB5" s="69"/>
+      <c r="EB5" s="75"/>
     </row>
     <row r="6" spans="1:132" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="67"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="34"/>
       <c r="J6" s="31" t="s">
         <v>192</v>
@@ -3375,145 +3378,145 @@
       <c r="K6" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="L6" s="95" t="s">
+      <c r="L6" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="97"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
       <c r="P6" s="35"/>
       <c r="Q6" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="R6" s="99"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="68"/>
-      <c r="Z6" s="68"/>
-      <c r="AA6" s="68"/>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="67"/>
-      <c r="AF6" s="66"/>
-      <c r="AG6" s="68"/>
-      <c r="AH6" s="68"/>
-      <c r="AI6" s="68"/>
-      <c r="AJ6" s="68"/>
-      <c r="AK6" s="68"/>
-      <c r="AL6" s="68"/>
-      <c r="AM6" s="68"/>
-      <c r="AN6" s="67"/>
-      <c r="AO6" s="70" t="s">
+      <c r="R6" s="85"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="83"/>
+      <c r="AA6" s="83"/>
+      <c r="AB6" s="83"/>
+      <c r="AC6" s="83"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="84"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="83"/>
+      <c r="AI6" s="83"/>
+      <c r="AJ6" s="83"/>
+      <c r="AK6" s="83"/>
+      <c r="AL6" s="83"/>
+      <c r="AM6" s="83"/>
+      <c r="AN6" s="84"/>
+      <c r="AO6" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="AP6" s="71"/>
+      <c r="AP6" s="116"/>
       <c r="AQ6" s="11"/>
       <c r="AR6" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="AS6" s="66"/>
-      <c r="AT6" s="68"/>
-      <c r="AU6" s="68"/>
-      <c r="AV6" s="68"/>
-      <c r="AW6" s="68"/>
-      <c r="AX6" s="68"/>
-      <c r="AY6" s="68"/>
-      <c r="AZ6" s="68"/>
-      <c r="BA6" s="68"/>
-      <c r="BB6" s="68"/>
-      <c r="BC6" s="68"/>
-      <c r="BD6" s="68"/>
-      <c r="BE6" s="68"/>
-      <c r="BF6" s="68"/>
-      <c r="BG6" s="68"/>
-      <c r="BH6" s="68"/>
-      <c r="BI6" s="67"/>
-      <c r="BJ6" s="66"/>
-      <c r="BK6" s="68"/>
-      <c r="BL6" s="68"/>
-      <c r="BM6" s="68"/>
-      <c r="BN6" s="68"/>
-      <c r="BO6" s="68"/>
-      <c r="BP6" s="68"/>
-      <c r="BQ6" s="68"/>
-      <c r="BR6" s="67"/>
-      <c r="BS6" s="70" t="s">
+      <c r="AS6" s="82"/>
+      <c r="AT6" s="83"/>
+      <c r="AU6" s="83"/>
+      <c r="AV6" s="83"/>
+      <c r="AW6" s="83"/>
+      <c r="AX6" s="83"/>
+      <c r="AY6" s="83"/>
+      <c r="AZ6" s="83"/>
+      <c r="BA6" s="83"/>
+      <c r="BB6" s="83"/>
+      <c r="BC6" s="83"/>
+      <c r="BD6" s="83"/>
+      <c r="BE6" s="83"/>
+      <c r="BF6" s="83"/>
+      <c r="BG6" s="83"/>
+      <c r="BH6" s="83"/>
+      <c r="BI6" s="84"/>
+      <c r="BJ6" s="82"/>
+      <c r="BK6" s="83"/>
+      <c r="BL6" s="83"/>
+      <c r="BM6" s="83"/>
+      <c r="BN6" s="83"/>
+      <c r="BO6" s="83"/>
+      <c r="BP6" s="83"/>
+      <c r="BQ6" s="83"/>
+      <c r="BR6" s="84"/>
+      <c r="BS6" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="BT6" s="84"/>
-      <c r="BU6" s="66"/>
-      <c r="BV6" s="68"/>
-      <c r="BW6" s="68"/>
-      <c r="BX6" s="68"/>
-      <c r="BY6" s="67"/>
-      <c r="BZ6" s="66"/>
-      <c r="CA6" s="67"/>
-      <c r="CB6" s="70" t="s">
+      <c r="BT6" s="100"/>
+      <c r="BU6" s="82"/>
+      <c r="BV6" s="83"/>
+      <c r="BW6" s="83"/>
+      <c r="BX6" s="83"/>
+      <c r="BY6" s="84"/>
+      <c r="BZ6" s="82"/>
+      <c r="CA6" s="84"/>
+      <c r="CB6" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="CC6" s="84"/>
-      <c r="CD6" s="66"/>
-      <c r="CE6" s="68"/>
-      <c r="CF6" s="67"/>
-      <c r="CG6" s="66" t="s">
+      <c r="CC6" s="100"/>
+      <c r="CD6" s="82"/>
+      <c r="CE6" s="83"/>
+      <c r="CF6" s="84"/>
+      <c r="CG6" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="CH6" s="73"/>
-      <c r="CI6" s="73"/>
-      <c r="CJ6" s="73"/>
-      <c r="CK6" s="73"/>
-      <c r="CL6" s="73"/>
-      <c r="CM6" s="73"/>
-      <c r="CN6" s="73"/>
-      <c r="CO6" s="73"/>
-      <c r="CP6" s="73"/>
-      <c r="CQ6" s="73"/>
-      <c r="CR6" s="73"/>
-      <c r="CS6" s="73"/>
-      <c r="CT6" s="73"/>
-      <c r="CU6" s="73"/>
-      <c r="CV6" s="73"/>
-      <c r="CW6" s="73"/>
-      <c r="CX6" s="73"/>
-      <c r="CY6" s="73"/>
-      <c r="CZ6" s="73"/>
-      <c r="DA6" s="73"/>
-      <c r="DB6" s="73"/>
-      <c r="DC6" s="73"/>
-      <c r="DD6" s="73"/>
-      <c r="DE6" s="73"/>
-      <c r="DF6" s="73"/>
-      <c r="DG6" s="73"/>
-      <c r="DH6" s="73"/>
-      <c r="DI6" s="74"/>
-      <c r="DJ6" s="70" t="s">
+      <c r="CH6" s="89"/>
+      <c r="CI6" s="89"/>
+      <c r="CJ6" s="89"/>
+      <c r="CK6" s="89"/>
+      <c r="CL6" s="89"/>
+      <c r="CM6" s="89"/>
+      <c r="CN6" s="89"/>
+      <c r="CO6" s="89"/>
+      <c r="CP6" s="89"/>
+      <c r="CQ6" s="89"/>
+      <c r="CR6" s="89"/>
+      <c r="CS6" s="89"/>
+      <c r="CT6" s="89"/>
+      <c r="CU6" s="89"/>
+      <c r="CV6" s="89"/>
+      <c r="CW6" s="89"/>
+      <c r="CX6" s="89"/>
+      <c r="CY6" s="89"/>
+      <c r="CZ6" s="89"/>
+      <c r="DA6" s="89"/>
+      <c r="DB6" s="89"/>
+      <c r="DC6" s="89"/>
+      <c r="DD6" s="89"/>
+      <c r="DE6" s="89"/>
+      <c r="DF6" s="89"/>
+      <c r="DG6" s="89"/>
+      <c r="DH6" s="89"/>
+      <c r="DI6" s="79"/>
+      <c r="DJ6" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="DK6" s="71"/>
-      <c r="DL6" s="71"/>
-      <c r="DM6" s="71"/>
-      <c r="DN6" s="71"/>
-      <c r="DO6" s="71"/>
-      <c r="DP6" s="71"/>
-      <c r="DQ6" s="71"/>
-      <c r="DR6" s="71"/>
-      <c r="DS6" s="71"/>
-      <c r="DT6" s="71"/>
-      <c r="DU6" s="71"/>
-      <c r="DV6" s="72" t="s">
+      <c r="DK6" s="116"/>
+      <c r="DL6" s="116"/>
+      <c r="DM6" s="116"/>
+      <c r="DN6" s="116"/>
+      <c r="DO6" s="116"/>
+      <c r="DP6" s="116"/>
+      <c r="DQ6" s="116"/>
+      <c r="DR6" s="116"/>
+      <c r="DS6" s="116"/>
+      <c r="DT6" s="116"/>
+      <c r="DU6" s="116"/>
+      <c r="DV6" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="DW6" s="73"/>
-      <c r="DX6" s="73"/>
-      <c r="DY6" s="73"/>
-      <c r="DZ6" s="73"/>
-      <c r="EA6" s="73"/>
-      <c r="EB6" s="74"/>
+      <c r="DW6" s="89"/>
+      <c r="DX6" s="89"/>
+      <c r="DY6" s="89"/>
+      <c r="DZ6" s="89"/>
+      <c r="EA6" s="89"/>
+      <c r="EB6" s="79"/>
     </row>
     <row r="7" spans="1:132" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -3526,575 +3529,575 @@
         <v>188</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="74" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="57" t="s">
+      <c r="I7" s="117"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="115"/>
+      <c r="V7" s="115"/>
+      <c r="W7" s="115"/>
+      <c r="X7" s="115"/>
+      <c r="Y7" s="115"/>
+      <c r="Z7" s="115"/>
+      <c r="AA7" s="120"/>
+      <c r="AB7" s="74" t="s">
         <v>188</v>
       </c>
-      <c r="AC7" s="74"/>
-      <c r="AD7" s="57"/>
-      <c r="AE7" s="59"/>
-      <c r="AF7" s="92" t="s">
+      <c r="AC7" s="79"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="120"/>
+      <c r="AF7" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="AG7" s="84"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="59"/>
+      <c r="AG7" s="100"/>
+      <c r="AH7" s="74"/>
+      <c r="AI7" s="120"/>
       <c r="AJ7" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="AK7" s="57"/>
-      <c r="AL7" s="58"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="58"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="58"/>
-      <c r="AW7" s="58"/>
-      <c r="AX7" s="58"/>
-      <c r="AY7" s="58"/>
-      <c r="AZ7" s="58"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="58"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="58"/>
-      <c r="BE7" s="58"/>
-      <c r="BF7" s="58"/>
-      <c r="BG7" s="58"/>
-      <c r="BH7" s="58"/>
-      <c r="BI7" s="59"/>
-      <c r="BJ7" s="57"/>
-      <c r="BK7" s="58"/>
-      <c r="BL7" s="58"/>
-      <c r="BM7" s="58"/>
-      <c r="BN7" s="58"/>
-      <c r="BO7" s="58"/>
-      <c r="BP7" s="58"/>
-      <c r="BQ7" s="58"/>
-      <c r="BR7" s="58"/>
-      <c r="BS7" s="58"/>
-      <c r="BT7" s="59"/>
-      <c r="BU7" s="57"/>
-      <c r="BV7" s="58"/>
-      <c r="BW7" s="58"/>
-      <c r="BX7" s="58"/>
-      <c r="BY7" s="59"/>
-      <c r="BZ7" s="57"/>
-      <c r="CA7" s="58"/>
-      <c r="CB7" s="58"/>
-      <c r="CC7" s="58"/>
-      <c r="CD7" s="58"/>
-      <c r="CE7" s="58"/>
-      <c r="CF7" s="58"/>
-      <c r="CG7" s="59"/>
-      <c r="CH7" s="57"/>
-      <c r="CI7" s="58"/>
-      <c r="CJ7" s="58"/>
-      <c r="CK7" s="58"/>
-      <c r="CL7" s="58"/>
-      <c r="CM7" s="58"/>
-      <c r="CN7" s="58"/>
-      <c r="CO7" s="58"/>
-      <c r="CP7" s="58"/>
-      <c r="CQ7" s="58"/>
-      <c r="CR7" s="58"/>
-      <c r="CS7" s="58"/>
-      <c r="CT7" s="58"/>
-      <c r="CU7" s="58"/>
-      <c r="CV7" s="58"/>
-      <c r="CW7" s="58"/>
-      <c r="CX7" s="58"/>
-      <c r="CY7" s="58"/>
-      <c r="CZ7" s="58"/>
-      <c r="DA7" s="58"/>
-      <c r="DB7" s="58"/>
-      <c r="DC7" s="58"/>
-      <c r="DD7" s="58"/>
-      <c r="DE7" s="58"/>
-      <c r="DF7" s="58"/>
-      <c r="DG7" s="58"/>
-      <c r="DH7" s="58"/>
-      <c r="DI7" s="59"/>
-      <c r="DJ7" s="57"/>
-      <c r="DK7" s="58"/>
-      <c r="DL7" s="58"/>
-      <c r="DM7" s="58"/>
-      <c r="DN7" s="58"/>
-      <c r="DO7" s="58"/>
-      <c r="DP7" s="58"/>
-      <c r="DQ7" s="58"/>
-      <c r="DR7" s="58"/>
-      <c r="DS7" s="58"/>
-      <c r="DT7" s="58"/>
-      <c r="DU7" s="59"/>
-      <c r="DV7" s="57"/>
-      <c r="DW7" s="58"/>
-      <c r="DX7" s="58"/>
-      <c r="DY7" s="58"/>
-      <c r="DZ7" s="58"/>
-      <c r="EA7" s="58"/>
-      <c r="EB7" s="59"/>
+      <c r="AK7" s="74"/>
+      <c r="AL7" s="115"/>
+      <c r="AM7" s="115"/>
+      <c r="AN7" s="115"/>
+      <c r="AO7" s="115"/>
+      <c r="AP7" s="115"/>
+      <c r="AQ7" s="115"/>
+      <c r="AR7" s="115"/>
+      <c r="AS7" s="115"/>
+      <c r="AT7" s="115"/>
+      <c r="AU7" s="115"/>
+      <c r="AV7" s="115"/>
+      <c r="AW7" s="115"/>
+      <c r="AX7" s="115"/>
+      <c r="AY7" s="115"/>
+      <c r="AZ7" s="115"/>
+      <c r="BA7" s="115"/>
+      <c r="BB7" s="115"/>
+      <c r="BC7" s="115"/>
+      <c r="BD7" s="115"/>
+      <c r="BE7" s="115"/>
+      <c r="BF7" s="115"/>
+      <c r="BG7" s="115"/>
+      <c r="BH7" s="115"/>
+      <c r="BI7" s="120"/>
+      <c r="BJ7" s="74"/>
+      <c r="BK7" s="115"/>
+      <c r="BL7" s="115"/>
+      <c r="BM7" s="115"/>
+      <c r="BN7" s="115"/>
+      <c r="BO7" s="115"/>
+      <c r="BP7" s="115"/>
+      <c r="BQ7" s="115"/>
+      <c r="BR7" s="115"/>
+      <c r="BS7" s="115"/>
+      <c r="BT7" s="120"/>
+      <c r="BU7" s="74"/>
+      <c r="BV7" s="115"/>
+      <c r="BW7" s="115"/>
+      <c r="BX7" s="115"/>
+      <c r="BY7" s="120"/>
+      <c r="BZ7" s="74"/>
+      <c r="CA7" s="115"/>
+      <c r="CB7" s="115"/>
+      <c r="CC7" s="115"/>
+      <c r="CD7" s="115"/>
+      <c r="CE7" s="115"/>
+      <c r="CF7" s="115"/>
+      <c r="CG7" s="120"/>
+      <c r="CH7" s="74"/>
+      <c r="CI7" s="115"/>
+      <c r="CJ7" s="115"/>
+      <c r="CK7" s="115"/>
+      <c r="CL7" s="115"/>
+      <c r="CM7" s="115"/>
+      <c r="CN7" s="115"/>
+      <c r="CO7" s="115"/>
+      <c r="CP7" s="115"/>
+      <c r="CQ7" s="115"/>
+      <c r="CR7" s="115"/>
+      <c r="CS7" s="115"/>
+      <c r="CT7" s="115"/>
+      <c r="CU7" s="115"/>
+      <c r="CV7" s="115"/>
+      <c r="CW7" s="115"/>
+      <c r="CX7" s="115"/>
+      <c r="CY7" s="115"/>
+      <c r="CZ7" s="115"/>
+      <c r="DA7" s="115"/>
+      <c r="DB7" s="115"/>
+      <c r="DC7" s="115"/>
+      <c r="DD7" s="115"/>
+      <c r="DE7" s="115"/>
+      <c r="DF7" s="115"/>
+      <c r="DG7" s="115"/>
+      <c r="DH7" s="115"/>
+      <c r="DI7" s="120"/>
+      <c r="DJ7" s="74"/>
+      <c r="DK7" s="115"/>
+      <c r="DL7" s="115"/>
+      <c r="DM7" s="115"/>
+      <c r="DN7" s="115"/>
+      <c r="DO7" s="115"/>
+      <c r="DP7" s="115"/>
+      <c r="DQ7" s="115"/>
+      <c r="DR7" s="115"/>
+      <c r="DS7" s="115"/>
+      <c r="DT7" s="115"/>
+      <c r="DU7" s="120"/>
+      <c r="DV7" s="74"/>
+      <c r="DW7" s="115"/>
+      <c r="DX7" s="115"/>
+      <c r="DY7" s="115"/>
+      <c r="DZ7" s="115"/>
+      <c r="EA7" s="115"/>
+      <c r="EB7" s="120"/>
     </row>
     <row r="8" spans="1:132" s="39" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B8" s="124">
+        <v>267</v>
+      </c>
+      <c r="B8" s="71">
         <v>1</v>
       </c>
-      <c r="C8" s="124">
+      <c r="C8" s="71">
         <v>2</v>
       </c>
-      <c r="D8" s="124">
+      <c r="D8" s="71">
         <v>3</v>
       </c>
-      <c r="E8" s="124">
+      <c r="E8" s="71">
         <v>4</v>
       </c>
-      <c r="F8" s="124">
+      <c r="F8" s="71">
         <v>5</v>
       </c>
-      <c r="G8" s="124">
+      <c r="G8" s="71">
         <v>6</v>
       </c>
-      <c r="H8" s="124">
+      <c r="H8" s="71">
         <v>7</v>
       </c>
-      <c r="I8" s="124">
+      <c r="I8" s="71">
         <v>8</v>
       </c>
-      <c r="J8" s="124">
+      <c r="J8" s="71">
         <v>9</v>
       </c>
-      <c r="K8" s="124">
+      <c r="K8" s="71">
         <v>10</v>
       </c>
-      <c r="L8" s="124">
+      <c r="L8" s="71">
         <v>11</v>
       </c>
-      <c r="M8" s="124">
+      <c r="M8" s="71">
         <v>12</v>
       </c>
-      <c r="N8" s="124">
+      <c r="N8" s="71">
         <v>13</v>
       </c>
-      <c r="O8" s="124">
+      <c r="O8" s="71">
         <v>14</v>
       </c>
-      <c r="P8" s="124">
+      <c r="P8" s="71">
         <v>15</v>
       </c>
-      <c r="Q8" s="124">
+      <c r="Q8" s="71">
         <v>16</v>
       </c>
-      <c r="R8" s="124">
+      <c r="R8" s="71">
         <v>17</v>
       </c>
-      <c r="S8" s="124">
+      <c r="S8" s="71">
         <v>18</v>
       </c>
-      <c r="T8" s="124">
+      <c r="T8" s="71">
         <v>19</v>
       </c>
-      <c r="U8" s="124">
+      <c r="U8" s="71">
         <v>20</v>
       </c>
-      <c r="V8" s="124">
+      <c r="V8" s="71">
         <v>21</v>
       </c>
-      <c r="W8" s="124">
+      <c r="W8" s="71">
         <v>22</v>
       </c>
-      <c r="X8" s="124">
+      <c r="X8" s="71">
         <v>23</v>
       </c>
-      <c r="Y8" s="124">
+      <c r="Y8" s="71">
         <v>24</v>
       </c>
-      <c r="Z8" s="124">
+      <c r="Z8" s="71">
         <v>25</v>
       </c>
-      <c r="AA8" s="124">
+      <c r="AA8" s="71">
         <v>26</v>
       </c>
-      <c r="AB8" s="124">
+      <c r="AB8" s="71">
         <v>27</v>
       </c>
-      <c r="AC8" s="124">
+      <c r="AC8" s="71">
         <v>28</v>
       </c>
-      <c r="AD8" s="124">
+      <c r="AD8" s="71">
         <v>29</v>
       </c>
-      <c r="AE8" s="124">
+      <c r="AE8" s="71">
         <v>30</v>
       </c>
-      <c r="AF8" s="124">
+      <c r="AF8" s="71">
         <v>31</v>
       </c>
-      <c r="AG8" s="124">
+      <c r="AG8" s="71">
         <v>32</v>
       </c>
-      <c r="AH8" s="124">
+      <c r="AH8" s="71">
         <v>33</v>
       </c>
-      <c r="AI8" s="124">
+      <c r="AI8" s="71">
         <v>34</v>
       </c>
-      <c r="AJ8" s="124">
+      <c r="AJ8" s="71">
         <v>35</v>
       </c>
-      <c r="AK8" s="124">
+      <c r="AK8" s="71">
         <v>36</v>
       </c>
-      <c r="AL8" s="124">
+      <c r="AL8" s="71">
         <v>37</v>
       </c>
-      <c r="AM8" s="124">
+      <c r="AM8" s="71">
         <v>38</v>
       </c>
-      <c r="AN8" s="124">
+      <c r="AN8" s="71">
         <v>39</v>
       </c>
-      <c r="AO8" s="124">
+      <c r="AO8" s="71">
         <v>40</v>
       </c>
-      <c r="AP8" s="124">
+      <c r="AP8" s="71">
         <v>41</v>
       </c>
-      <c r="AQ8" s="124">
+      <c r="AQ8" s="71">
         <v>42</v>
       </c>
-      <c r="AR8" s="124">
+      <c r="AR8" s="71">
         <v>43</v>
       </c>
-      <c r="AS8" s="124">
+      <c r="AS8" s="71">
         <v>44</v>
       </c>
-      <c r="AT8" s="124">
+      <c r="AT8" s="71">
         <v>45</v>
       </c>
-      <c r="AU8" s="124">
+      <c r="AU8" s="71">
         <v>46</v>
       </c>
-      <c r="AV8" s="124">
+      <c r="AV8" s="71">
         <v>47</v>
       </c>
-      <c r="AW8" s="124">
+      <c r="AW8" s="71">
         <v>48</v>
       </c>
-      <c r="AX8" s="124">
+      <c r="AX8" s="71">
         <v>49</v>
       </c>
-      <c r="AY8" s="124">
+      <c r="AY8" s="71">
         <v>50</v>
       </c>
-      <c r="AZ8" s="124">
+      <c r="AZ8" s="71">
         <v>51</v>
       </c>
-      <c r="BA8" s="124">
+      <c r="BA8" s="71">
         <v>52</v>
       </c>
-      <c r="BB8" s="124">
+      <c r="BB8" s="71">
         <v>53</v>
       </c>
-      <c r="BC8" s="124">
+      <c r="BC8" s="71">
         <v>54</v>
       </c>
-      <c r="BD8" s="124">
+      <c r="BD8" s="71">
         <v>55</v>
       </c>
-      <c r="BE8" s="124">
+      <c r="BE8" s="71">
         <v>56</v>
       </c>
-      <c r="BF8" s="124">
+      <c r="BF8" s="71">
         <v>57</v>
       </c>
-      <c r="BG8" s="124">
+      <c r="BG8" s="71">
         <v>58</v>
       </c>
-      <c r="BH8" s="124">
+      <c r="BH8" s="71">
         <v>59</v>
       </c>
-      <c r="BI8" s="124">
+      <c r="BI8" s="71">
         <v>60</v>
       </c>
-      <c r="BJ8" s="124">
+      <c r="BJ8" s="71">
         <v>61</v>
       </c>
-      <c r="BK8" s="124">
+      <c r="BK8" s="71">
         <v>62</v>
       </c>
-      <c r="BL8" s="124">
+      <c r="BL8" s="71">
         <v>63</v>
       </c>
-      <c r="BM8" s="124">
+      <c r="BM8" s="71">
         <v>64</v>
       </c>
-      <c r="BN8" s="124">
+      <c r="BN8" s="71">
         <v>65</v>
       </c>
-      <c r="BO8" s="124">
+      <c r="BO8" s="71">
         <v>66</v>
       </c>
-      <c r="BP8" s="124">
+      <c r="BP8" s="71">
         <v>67</v>
       </c>
-      <c r="BQ8" s="124">
+      <c r="BQ8" s="71">
         <v>68</v>
       </c>
-      <c r="BR8" s="124">
+      <c r="BR8" s="71">
         <v>69</v>
       </c>
-      <c r="BS8" s="124">
+      <c r="BS8" s="71">
         <v>70</v>
       </c>
-      <c r="BT8" s="124">
+      <c r="BT8" s="71">
         <v>71</v>
       </c>
-      <c r="BU8" s="124">
+      <c r="BU8" s="71">
         <v>72</v>
       </c>
-      <c r="BV8" s="124">
+      <c r="BV8" s="71">
         <v>73</v>
       </c>
-      <c r="BW8" s="124">
+      <c r="BW8" s="71">
         <v>74</v>
       </c>
-      <c r="BX8" s="124">
+      <c r="BX8" s="71">
         <v>75</v>
       </c>
-      <c r="BY8" s="124">
+      <c r="BY8" s="71">
         <v>76</v>
       </c>
-      <c r="BZ8" s="124">
+      <c r="BZ8" s="71">
         <v>77</v>
       </c>
-      <c r="CA8" s="124">
+      <c r="CA8" s="71">
         <v>78</v>
       </c>
-      <c r="CB8" s="124">
+      <c r="CB8" s="71">
         <v>79</v>
       </c>
-      <c r="CC8" s="124">
+      <c r="CC8" s="71">
         <v>80</v>
       </c>
-      <c r="CD8" s="124">
+      <c r="CD8" s="71">
         <v>81</v>
       </c>
-      <c r="CE8" s="124">
+      <c r="CE8" s="71">
         <v>82</v>
       </c>
-      <c r="CF8" s="124">
+      <c r="CF8" s="71">
         <v>83</v>
       </c>
-      <c r="CG8" s="124">
+      <c r="CG8" s="71">
         <v>84</v>
       </c>
-      <c r="CH8" s="124">
+      <c r="CH8" s="71">
         <v>85</v>
       </c>
-      <c r="CI8" s="124">
+      <c r="CI8" s="71">
         <v>86</v>
       </c>
-      <c r="CJ8" s="124">
+      <c r="CJ8" s="71">
         <v>87</v>
       </c>
-      <c r="CK8" s="124">
+      <c r="CK8" s="71">
         <v>88</v>
       </c>
-      <c r="CL8" s="124">
+      <c r="CL8" s="71">
         <v>89</v>
       </c>
-      <c r="CM8" s="124">
+      <c r="CM8" s="71">
         <v>90</v>
       </c>
-      <c r="CN8" s="124">
+      <c r="CN8" s="71">
         <v>91</v>
       </c>
-      <c r="CO8" s="124">
+      <c r="CO8" s="71">
         <v>92</v>
       </c>
-      <c r="CP8" s="124">
+      <c r="CP8" s="71">
         <v>93</v>
       </c>
-      <c r="CQ8" s="124">
+      <c r="CQ8" s="71">
         <v>94</v>
       </c>
-      <c r="CR8" s="124">
+      <c r="CR8" s="71">
         <v>95</v>
       </c>
-      <c r="CS8" s="124">
+      <c r="CS8" s="71">
         <v>96</v>
       </c>
-      <c r="CT8" s="124">
+      <c r="CT8" s="71">
         <v>97</v>
       </c>
-      <c r="CU8" s="124">
+      <c r="CU8" s="71">
         <v>98</v>
       </c>
-      <c r="CV8" s="124">
+      <c r="CV8" s="71">
         <v>99</v>
       </c>
-      <c r="CW8" s="124">
+      <c r="CW8" s="71">
         <v>100</v>
       </c>
-      <c r="CX8" s="124">
+      <c r="CX8" s="71">
         <v>101</v>
       </c>
-      <c r="CY8" s="124">
+      <c r="CY8" s="71">
         <v>102</v>
       </c>
-      <c r="CZ8" s="124">
+      <c r="CZ8" s="71">
         <v>103</v>
       </c>
-      <c r="DA8" s="124">
+      <c r="DA8" s="71">
         <v>104</v>
       </c>
-      <c r="DB8" s="124">
+      <c r="DB8" s="71">
         <v>105</v>
       </c>
-      <c r="DC8" s="124">
+      <c r="DC8" s="71">
         <v>106</v>
       </c>
-      <c r="DD8" s="124">
+      <c r="DD8" s="71">
         <v>107</v>
       </c>
-      <c r="DE8" s="124">
+      <c r="DE8" s="71">
         <v>108</v>
       </c>
-      <c r="DF8" s="124">
+      <c r="DF8" s="71">
         <v>109</v>
       </c>
-      <c r="DG8" s="124">
+      <c r="DG8" s="71">
         <v>110</v>
       </c>
-      <c r="DH8" s="124">
+      <c r="DH8" s="71">
         <v>111</v>
       </c>
-      <c r="DI8" s="124">
+      <c r="DI8" s="71">
         <v>112</v>
       </c>
-      <c r="DJ8" s="124">
+      <c r="DJ8" s="71">
         <v>113</v>
       </c>
-      <c r="DK8" s="124">
+      <c r="DK8" s="71">
         <v>114</v>
       </c>
-      <c r="DL8" s="124">
+      <c r="DL8" s="71">
         <v>115</v>
       </c>
-      <c r="DM8" s="124">
+      <c r="DM8" s="71">
         <v>116</v>
       </c>
-      <c r="DN8" s="124">
+      <c r="DN8" s="71">
         <v>117</v>
       </c>
-      <c r="DO8" s="124">
+      <c r="DO8" s="71">
         <v>118</v>
       </c>
-      <c r="DP8" s="124">
+      <c r="DP8" s="71">
         <v>119</v>
       </c>
-      <c r="DQ8" s="124">
+      <c r="DQ8" s="71">
         <v>120</v>
       </c>
-      <c r="DR8" s="124">
+      <c r="DR8" s="71">
         <v>121</v>
       </c>
-      <c r="DS8" s="124">
+      <c r="DS8" s="71">
         <v>122</v>
       </c>
-      <c r="DT8" s="124">
+      <c r="DT8" s="71">
         <v>123</v>
       </c>
-      <c r="DU8" s="124">
+      <c r="DU8" s="71">
         <v>124</v>
       </c>
-      <c r="DV8" s="124">
+      <c r="DV8" s="71">
         <v>125</v>
       </c>
-      <c r="DW8" s="124">
+      <c r="DW8" s="71">
         <v>126</v>
       </c>
-      <c r="DX8" s="124">
+      <c r="DX8" s="71">
         <v>127</v>
       </c>
-      <c r="DY8" s="124">
+      <c r="DY8" s="71">
         <v>128</v>
       </c>
-      <c r="DZ8" s="124">
+      <c r="DZ8" s="71">
         <v>129</v>
       </c>
-      <c r="EA8" s="124">
+      <c r="EA8" s="71">
         <v>130</v>
       </c>
-      <c r="EB8" s="124">
+      <c r="EB8" s="71">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="T6:AE6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="CQ3:CS3"/>
-    <mergeCell ref="BO4:BR4"/>
-    <mergeCell ref="BX4:BY4"/>
-    <mergeCell ref="BL5:BM5"/>
-    <mergeCell ref="BO5:BR5"/>
-    <mergeCell ref="BW5:BY5"/>
-    <mergeCell ref="CH5:CI5"/>
-    <mergeCell ref="CD5:CF5"/>
-    <mergeCell ref="BZ1:CG1"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="CB6:CC6"/>
-    <mergeCell ref="BK3:BN3"/>
-    <mergeCell ref="CN3:CP3"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="T1:AE1"/>
-    <mergeCell ref="AF1:BI1"/>
-    <mergeCell ref="BJ1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="DV1:EB1"/>
+    <mergeCell ref="DV7:EB7"/>
+    <mergeCell ref="AT5:AW5"/>
+    <mergeCell ref="AX5:BA5"/>
+    <mergeCell ref="BB5:BE5"/>
+    <mergeCell ref="BF5:BI5"/>
+    <mergeCell ref="BJ7:BT7"/>
+    <mergeCell ref="BU7:BY7"/>
+    <mergeCell ref="BZ7:CG7"/>
+    <mergeCell ref="CH7:DI7"/>
+    <mergeCell ref="DJ7:DU7"/>
+    <mergeCell ref="BZ6:CA6"/>
+    <mergeCell ref="BU6:BY6"/>
+    <mergeCell ref="BJ6:BR6"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AK7:BI7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="CH1:DI1"/>
+    <mergeCell ref="DJ1:DU1"/>
+    <mergeCell ref="AS6:BI6"/>
+    <mergeCell ref="AF6:AN6"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DR5:DS5"/>
+    <mergeCell ref="CD6:CF6"/>
+    <mergeCell ref="DJ6:DU6"/>
+    <mergeCell ref="AF5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="DD5:DE5"/>
+    <mergeCell ref="DH5:DI5"/>
+    <mergeCell ref="DJ5:DK5"/>
+    <mergeCell ref="AO6:AP6"/>
     <mergeCell ref="DV6:EB6"/>
     <mergeCell ref="CF4:CG4"/>
     <mergeCell ref="CJ4:CK4"/>
@@ -4111,41 +4114,41 @@
     <mergeCell ref="DK4:DL4"/>
     <mergeCell ref="CX5:CZ5"/>
     <mergeCell ref="DA5:DB5"/>
-    <mergeCell ref="AS6:BI6"/>
-    <mergeCell ref="AF6:AN6"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DR5:DS5"/>
-    <mergeCell ref="CD6:CF6"/>
-    <mergeCell ref="DJ6:DU6"/>
-    <mergeCell ref="AF5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="DD5:DE5"/>
-    <mergeCell ref="DH5:DI5"/>
-    <mergeCell ref="DJ5:DK5"/>
-    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="AF1:BI1"/>
+    <mergeCell ref="BJ1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CG1"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="CB6:CC6"/>
+    <mergeCell ref="BK3:BN3"/>
+    <mergeCell ref="CN3:CP3"/>
+    <mergeCell ref="CQ3:CS3"/>
+    <mergeCell ref="BO4:BR4"/>
+    <mergeCell ref="BX4:BY4"/>
+    <mergeCell ref="BL5:BM5"/>
+    <mergeCell ref="BO5:BR5"/>
+    <mergeCell ref="BW5:BY5"/>
+    <mergeCell ref="CH5:CI5"/>
+    <mergeCell ref="CD5:CF5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="B6:H6"/>
     <mergeCell ref="I7:S7"/>
     <mergeCell ref="T7:AA7"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="T6:AE6"/>
+    <mergeCell ref="R6:S6"/>
     <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AK7:BI7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="CH1:DI1"/>
-    <mergeCell ref="DJ1:DU1"/>
-    <mergeCell ref="DV1:EB1"/>
-    <mergeCell ref="DV7:EB7"/>
-    <mergeCell ref="AT5:AW5"/>
-    <mergeCell ref="AX5:BA5"/>
-    <mergeCell ref="BB5:BE5"/>
-    <mergeCell ref="BF5:BI5"/>
-    <mergeCell ref="BJ7:BT7"/>
-    <mergeCell ref="BU7:BY7"/>
-    <mergeCell ref="BZ7:CG7"/>
-    <mergeCell ref="CH7:DI7"/>
-    <mergeCell ref="DJ7:DU7"/>
-    <mergeCell ref="BZ6:CA6"/>
-    <mergeCell ref="BU6:BY6"/>
-    <mergeCell ref="BJ6:BR6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AD4" r:id="rId1" xr:uid="{F3767099-F5B4-4A43-9EF8-725310DD37E5}"/>
@@ -4153,16 +4156,22 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4426,20 +4435,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E6DF85-604C-4C11-B168-A00921BCEA51}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF050CE3-396B-4D35-A168-28F84B0244F1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4465,25 +4482,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF050CE3-396B-4D35-A168-28F84B0244F1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E6DF85-604C-4C11-B168-A00921BCEA51}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{bf346810-9c7d-43de-a872-24a2ef3995a8}" enabled="0" method="" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" removed="1"/>
+  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" contentBits="3" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
feat: update sales resources (#2320)
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-sales-template-2024-25.xlsx
+++ b/public/files/bulk-upload-sales-template-2024-25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mhclg.sharepoint.com/sites/HousingandplanningandCOREstatistics/Shared Documents/CORE Lettings/01 Annual log changes/2024-25/03 Materials for providers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SamuelIvko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{CD602663-1CCE-42E7-A578-0D2CBA61949F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24C1F701-145D-49F7-B68D-47664BB64896}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7D1A7-CEC5-402E-A9C5-E5E0C01F6637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="4680" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="24-25 Sales template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="271">
   <si>
     <t>Section</t>
   </si>
@@ -823,12 +823,6 @@
 Yes, if the purchase was a staircasing transaction (if field 86 = 1)</t>
   </si>
   <si>
-    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or if a mortgage was not used (if field 103 = 2)</t>
-  </si>
-  <si>
-    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3), if a mortgage was not used (if field 103 = 2) or if 'Other' is not selected for mortgage lender name (if field 105 is not 40)</t>
-  </si>
-  <si>
     <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or the type of shared ownership sale is not Social Homebuy (if field 9 is not 18)</t>
   </si>
   <si>
@@ -865,6 +859,15 @@
   </si>
   <si>
     <t>Field number</t>
+  </si>
+  <si>
+    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or if a mortgage was not used (if field 103 = 2 or 3)</t>
+  </si>
+  <si>
+    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3), if a mortgage was not used (if field 103 = 2 or 3) or if 'Other' is not selected for mortgage lender name (if field 105 is not 40)</t>
+  </si>
+  <si>
+    <t>Yes, if the purchase was not made through a shared ownership scheme (if field 8 = 2 or 3) or if mortgage information is unknown (field 103 = 3)</t>
   </si>
 </sst>
 </file>
@@ -1428,66 +1431,167 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1497,136 +1601,35 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1851,7 +1854,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E14" sqref="E14"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1883,155 +1886,155 @@
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="81" t="s">
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="81"/>
-      <c r="V1" s="81"/>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="81"/>
-      <c r="Z1" s="81"/>
-      <c r="AA1" s="81"/>
-      <c r="AB1" s="81"/>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="56" t="s">
+      <c r="U1" s="106"/>
+      <c r="V1" s="106"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="106"/>
+      <c r="Y1" s="106"/>
+      <c r="Z1" s="106"/>
+      <c r="AA1" s="106"/>
+      <c r="AB1" s="106"/>
+      <c r="AC1" s="106"/>
+      <c r="AD1" s="106"/>
+      <c r="AE1" s="106"/>
+      <c r="AF1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="56"/>
-      <c r="AI1" s="56"/>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="56"/>
-      <c r="AL1" s="56"/>
-      <c r="AM1" s="56"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="56"/>
-      <c r="AQ1" s="56"/>
-      <c r="AR1" s="56"/>
-      <c r="AS1" s="56"/>
-      <c r="AT1" s="56"/>
-      <c r="AU1" s="56"/>
-      <c r="AV1" s="56"/>
-      <c r="AW1" s="56"/>
-      <c r="AX1" s="56"/>
-      <c r="AY1" s="56"/>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="56"/>
-      <c r="BB1" s="56"/>
-      <c r="BC1" s="56"/>
-      <c r="BD1" s="56"/>
-      <c r="BE1" s="56"/>
-      <c r="BF1" s="56"/>
-      <c r="BG1" s="56"/>
-      <c r="BH1" s="56"/>
-      <c r="BI1" s="56"/>
-      <c r="BJ1" s="82" t="s">
+      <c r="AG1" s="107"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="107"/>
+      <c r="AJ1" s="107"/>
+      <c r="AK1" s="107"/>
+      <c r="AL1" s="107"/>
+      <c r="AM1" s="107"/>
+      <c r="AN1" s="107"/>
+      <c r="AO1" s="107"/>
+      <c r="AP1" s="107"/>
+      <c r="AQ1" s="107"/>
+      <c r="AR1" s="107"/>
+      <c r="AS1" s="107"/>
+      <c r="AT1" s="107"/>
+      <c r="AU1" s="107"/>
+      <c r="AV1" s="107"/>
+      <c r="AW1" s="107"/>
+      <c r="AX1" s="107"/>
+      <c r="AY1" s="107"/>
+      <c r="AZ1" s="107"/>
+      <c r="BA1" s="107"/>
+      <c r="BB1" s="107"/>
+      <c r="BC1" s="107"/>
+      <c r="BD1" s="107"/>
+      <c r="BE1" s="107"/>
+      <c r="BF1" s="107"/>
+      <c r="BG1" s="107"/>
+      <c r="BH1" s="107"/>
+      <c r="BI1" s="107"/>
+      <c r="BJ1" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="BK1" s="82"/>
-      <c r="BL1" s="82"/>
-      <c r="BM1" s="82"/>
-      <c r="BN1" s="82"/>
-      <c r="BO1" s="82"/>
-      <c r="BP1" s="82"/>
-      <c r="BQ1" s="82"/>
-      <c r="BR1" s="82"/>
-      <c r="BS1" s="82"/>
-      <c r="BT1" s="82"/>
-      <c r="BU1" s="55" t="s">
+      <c r="BK1" s="108"/>
+      <c r="BL1" s="108"/>
+      <c r="BM1" s="108"/>
+      <c r="BN1" s="108"/>
+      <c r="BO1" s="108"/>
+      <c r="BP1" s="108"/>
+      <c r="BQ1" s="108"/>
+      <c r="BR1" s="108"/>
+      <c r="BS1" s="108"/>
+      <c r="BT1" s="108"/>
+      <c r="BU1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="BV1" s="55"/>
-      <c r="BW1" s="55"/>
-      <c r="BX1" s="55"/>
-      <c r="BY1" s="55"/>
-      <c r="BZ1" s="83" t="s">
+      <c r="BV1" s="109"/>
+      <c r="BW1" s="109"/>
+      <c r="BX1" s="109"/>
+      <c r="BY1" s="109"/>
+      <c r="BZ1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="CA1" s="83"/>
-      <c r="CB1" s="83"/>
-      <c r="CC1" s="83"/>
-      <c r="CD1" s="83"/>
-      <c r="CE1" s="83"/>
-      <c r="CF1" s="83"/>
-      <c r="CG1" s="83"/>
-      <c r="CH1" s="54" t="s">
+      <c r="CA1" s="98"/>
+      <c r="CB1" s="98"/>
+      <c r="CC1" s="98"/>
+      <c r="CD1" s="98"/>
+      <c r="CE1" s="98"/>
+      <c r="CF1" s="98"/>
+      <c r="CG1" s="98"/>
+      <c r="CH1" s="122" t="s">
         <v>7</v>
       </c>
-      <c r="CI1" s="54"/>
-      <c r="CJ1" s="54"/>
-      <c r="CK1" s="54"/>
-      <c r="CL1" s="54"/>
-      <c r="CM1" s="54"/>
-      <c r="CN1" s="54"/>
-      <c r="CO1" s="54"/>
-      <c r="CP1" s="54"/>
-      <c r="CQ1" s="54"/>
-      <c r="CR1" s="54"/>
-      <c r="CS1" s="54"/>
-      <c r="CT1" s="54"/>
-      <c r="CU1" s="54"/>
-      <c r="CV1" s="54"/>
-      <c r="CW1" s="54"/>
-      <c r="CX1" s="54"/>
-      <c r="CY1" s="54"/>
-      <c r="CZ1" s="54"/>
-      <c r="DA1" s="54"/>
-      <c r="DB1" s="54"/>
-      <c r="DC1" s="54"/>
-      <c r="DD1" s="54"/>
-      <c r="DE1" s="54"/>
-      <c r="DF1" s="54"/>
-      <c r="DG1" s="54"/>
-      <c r="DH1" s="54"/>
-      <c r="DI1" s="54"/>
-      <c r="DJ1" s="55" t="s">
+      <c r="CI1" s="122"/>
+      <c r="CJ1" s="122"/>
+      <c r="CK1" s="122"/>
+      <c r="CL1" s="122"/>
+      <c r="CM1" s="122"/>
+      <c r="CN1" s="122"/>
+      <c r="CO1" s="122"/>
+      <c r="CP1" s="122"/>
+      <c r="CQ1" s="122"/>
+      <c r="CR1" s="122"/>
+      <c r="CS1" s="122"/>
+      <c r="CT1" s="122"/>
+      <c r="CU1" s="122"/>
+      <c r="CV1" s="122"/>
+      <c r="CW1" s="122"/>
+      <c r="CX1" s="122"/>
+      <c r="CY1" s="122"/>
+      <c r="CZ1" s="122"/>
+      <c r="DA1" s="122"/>
+      <c r="DB1" s="122"/>
+      <c r="DC1" s="122"/>
+      <c r="DD1" s="122"/>
+      <c r="DE1" s="122"/>
+      <c r="DF1" s="122"/>
+      <c r="DG1" s="122"/>
+      <c r="DH1" s="122"/>
+      <c r="DI1" s="122"/>
+      <c r="DJ1" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="DK1" s="55"/>
-      <c r="DL1" s="55"/>
-      <c r="DM1" s="55"/>
-      <c r="DN1" s="55"/>
-      <c r="DO1" s="55"/>
-      <c r="DP1" s="55"/>
-      <c r="DQ1" s="55"/>
-      <c r="DR1" s="55"/>
-      <c r="DS1" s="55"/>
-      <c r="DT1" s="55"/>
-      <c r="DU1" s="55"/>
-      <c r="DV1" s="56" t="s">
+      <c r="DK1" s="109"/>
+      <c r="DL1" s="109"/>
+      <c r="DM1" s="109"/>
+      <c r="DN1" s="109"/>
+      <c r="DO1" s="109"/>
+      <c r="DP1" s="109"/>
+      <c r="DQ1" s="109"/>
+      <c r="DR1" s="109"/>
+      <c r="DS1" s="109"/>
+      <c r="DT1" s="109"/>
+      <c r="DU1" s="109"/>
+      <c r="DV1" s="107" t="s">
         <v>222</v>
       </c>
-      <c r="DW1" s="56"/>
-      <c r="DX1" s="56"/>
-      <c r="DY1" s="56"/>
-      <c r="DZ1" s="56"/>
-      <c r="EA1" s="56"/>
-      <c r="EB1" s="56"/>
+      <c r="DW1" s="107"/>
+      <c r="DX1" s="107"/>
+      <c r="DY1" s="107"/>
+      <c r="DZ1" s="107"/>
+      <c r="EA1" s="107"/>
+      <c r="EB1" s="107"/>
     </row>
     <row r="2" spans="1:132" ht="115" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2041,7 +2044,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
@@ -2431,271 +2434,271 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:132" s="121" customFormat="1" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:132" s="68" customFormat="1" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="70" t="s">
         <v>197</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="E3" s="101"/>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="102" t="s">
+      <c r="I3" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="K3" s="103" t="s">
+      <c r="K3" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="M3" s="104"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103"/>
-      <c r="P3" s="103" t="s">
+      <c r="M3" s="57"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56" t="s">
         <v>205</v>
       </c>
-      <c r="Q3" s="103"/>
-      <c r="R3" s="103" t="s">
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="S3" s="105" t="s">
-        <v>268</v>
-      </c>
-      <c r="T3" s="106" t="s">
+      <c r="S3" s="58" t="s">
+        <v>266</v>
+      </c>
+      <c r="T3" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="107" t="s">
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="106"/>
-      <c r="Z3" s="101"/>
-      <c r="AA3" s="101"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
       <c r="AB3" s="27" t="s">
         <v>211</v>
       </c>
       <c r="AC3" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="AD3" s="101"/>
-      <c r="AE3" s="103" t="s">
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="AF3" s="101" t="s">
+      <c r="AF3" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="AG3" s="101" t="s">
+      <c r="AG3" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="AH3" s="101"/>
-      <c r="AI3" s="108" t="s">
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="AJ3" s="106" t="s">
+      <c r="AJ3" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="AK3" s="109"/>
-      <c r="AL3" s="109"/>
-      <c r="AM3" s="109"/>
-      <c r="AN3" s="106" t="s">
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="62"/>
+      <c r="AM3" s="62"/>
+      <c r="AN3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="AO3" s="106"/>
-      <c r="AP3" s="108" t="s">
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="AQ3" s="106"/>
-      <c r="AR3" s="106"/>
-      <c r="AS3" s="106" t="s">
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="59"/>
+      <c r="AS3" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="AT3" s="106"/>
-      <c r="AU3" s="106"/>
-      <c r="AV3" s="106" t="s">
+      <c r="AT3" s="59"/>
+      <c r="AU3" s="59"/>
+      <c r="AV3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="AW3" s="106"/>
-      <c r="AX3" s="106"/>
-      <c r="AY3" s="106"/>
-      <c r="AZ3" s="106" t="s">
+      <c r="AW3" s="59"/>
+      <c r="AX3" s="59"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="BA3" s="106"/>
-      <c r="BB3" s="106"/>
-      <c r="BC3" s="106"/>
-      <c r="BD3" s="106" t="s">
+      <c r="BA3" s="59"/>
+      <c r="BB3" s="59"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="BE3" s="106"/>
-      <c r="BF3" s="106"/>
-      <c r="BG3" s="106"/>
-      <c r="BH3" s="106" t="s">
+      <c r="BE3" s="59"/>
+      <c r="BF3" s="59"/>
+      <c r="BG3" s="59"/>
+      <c r="BH3" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="BI3" s="106"/>
-      <c r="BJ3" s="101"/>
-      <c r="BK3" s="110" t="s">
+      <c r="BI3" s="59"/>
+      <c r="BJ3" s="54"/>
+      <c r="BK3" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="BL3" s="111"/>
-      <c r="BM3" s="111"/>
-      <c r="BN3" s="112"/>
-      <c r="BO3" s="113"/>
-      <c r="BP3" s="101"/>
-      <c r="BQ3" s="101"/>
-      <c r="BR3" s="114"/>
-      <c r="BS3" s="106"/>
-      <c r="BT3" s="106"/>
-      <c r="BU3" s="115" t="s">
+      <c r="BL3" s="102"/>
+      <c r="BM3" s="102"/>
+      <c r="BN3" s="103"/>
+      <c r="BO3" s="63"/>
+      <c r="BP3" s="54"/>
+      <c r="BQ3" s="54"/>
+      <c r="BR3" s="64"/>
+      <c r="BS3" s="59"/>
+      <c r="BT3" s="59"/>
+      <c r="BU3" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="BV3" s="115"/>
-      <c r="BW3" s="115" t="s">
+      <c r="BV3" s="65"/>
+      <c r="BW3" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="BX3" s="106" t="s">
+      <c r="BX3" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="BY3" s="106" t="s">
+      <c r="BY3" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="BZ3" s="106" t="s">
+      <c r="BZ3" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="CA3" s="106"/>
-      <c r="CB3" s="106" t="s">
+      <c r="CA3" s="59"/>
+      <c r="CB3" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="CC3" s="106"/>
-      <c r="CD3" s="106"/>
-      <c r="CE3" s="106" t="s">
+      <c r="CC3" s="59"/>
+      <c r="CD3" s="59"/>
+      <c r="CE3" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="CF3" s="106"/>
-      <c r="CG3" s="106" t="s">
+      <c r="CF3" s="59"/>
+      <c r="CG3" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="CH3" s="116" t="s">
+      <c r="CH3" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="CI3" s="106" t="s">
+      <c r="CI3" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="CJ3" s="106"/>
-      <c r="CK3" s="106"/>
-      <c r="CL3" s="106"/>
-      <c r="CM3" s="106" t="s">
+      <c r="CJ3" s="59"/>
+      <c r="CK3" s="59"/>
+      <c r="CL3" s="59"/>
+      <c r="CM3" s="59" t="s">
         <v>135</v>
       </c>
-      <c r="CN3" s="117" t="s">
+      <c r="CN3" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="CO3" s="118"/>
-      <c r="CP3" s="119"/>
-      <c r="CQ3" s="117" t="s">
+      <c r="CO3" s="91"/>
+      <c r="CP3" s="92"/>
+      <c r="CQ3" s="90" t="s">
         <v>137</v>
       </c>
-      <c r="CR3" s="118"/>
-      <c r="CS3" s="119"/>
-      <c r="CT3" s="106" t="s">
+      <c r="CR3" s="91"/>
+      <c r="CS3" s="92"/>
+      <c r="CT3" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="CU3" s="106" t="s">
+      <c r="CU3" s="59" t="s">
         <v>123</v>
       </c>
-      <c r="CV3" s="106"/>
-      <c r="CW3" s="106"/>
-      <c r="CX3" s="106" t="s">
+      <c r="CV3" s="59"/>
+      <c r="CW3" s="59"/>
+      <c r="CX3" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="CY3" s="107" t="s">
+      <c r="CY3" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="CZ3" s="122" t="s">
-        <v>267</v>
+      <c r="CZ3" s="69" t="s">
+        <v>265</v>
       </c>
       <c r="DA3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="DB3" s="106"/>
-      <c r="DC3" s="116"/>
-      <c r="DD3" s="116"/>
-      <c r="DE3" s="106" t="s">
+      <c r="DB3" s="59"/>
+      <c r="DC3" s="66"/>
+      <c r="DD3" s="66"/>
+      <c r="DE3" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="DF3" s="106" t="s">
+      <c r="DF3" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="DG3" s="106" t="s">
+      <c r="DG3" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="DH3" s="106" t="s">
+      <c r="DH3" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="DI3" s="106" t="s">
+      <c r="DI3" s="59" t="s">
         <v>144</v>
       </c>
-      <c r="DJ3" s="116"/>
-      <c r="DK3" s="106" t="s">
+      <c r="DJ3" s="66"/>
+      <c r="DK3" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="DL3" s="106" t="s">
+      <c r="DL3" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="DM3" s="101" t="s">
+      <c r="DM3" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="DN3" s="101"/>
+      <c r="DN3" s="54"/>
       <c r="DO3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="DP3" s="101"/>
-      <c r="DQ3" s="120"/>
-      <c r="DR3" s="120"/>
-      <c r="DS3" s="101" t="s">
+      <c r="DP3" s="54"/>
+      <c r="DQ3" s="67"/>
+      <c r="DR3" s="67"/>
+      <c r="DS3" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="DT3" s="101" t="s">
+      <c r="DT3" s="54" t="s">
         <v>148</v>
       </c>
-      <c r="DU3" s="101" t="s">
+      <c r="DU3" s="54" t="s">
         <v>144</v>
       </c>
       <c r="DV3" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="DW3" s="101"/>
+      <c r="DW3" s="54"/>
       <c r="DX3" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="DY3" s="120"/>
-      <c r="DZ3" s="101" t="s">
+      <c r="DY3" s="67"/>
+      <c r="DZ3" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="EA3" s="101" t="s">
+      <c r="EA3" s="54" t="s">
         <v>149</v>
       </c>
-      <c r="EB3" s="101" t="s">
+      <c r="EB3" s="54" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:132" s="51" customFormat="1" ht="125" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:132" s="51" customFormat="1" ht="137.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>150</v>
       </c>
@@ -2735,11 +2738,11 @@
       <c r="M4" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="N4" s="93" t="s">
+      <c r="N4" s="72" t="s">
         <v>158</v>
       </c>
-      <c r="O4" s="98"/>
-      <c r="P4" s="94"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="81"/>
       <c r="Q4" s="31" t="s">
         <v>153</v>
       </c>
@@ -2761,19 +2764,19 @@
       <c r="W4" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="X4" s="57" t="s">
+      <c r="X4" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="Y4" s="69"/>
-      <c r="Z4" s="89" t="s">
+      <c r="Y4" s="75"/>
+      <c r="Z4" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="AA4" s="91"/>
+      <c r="AA4" s="73"/>
       <c r="AB4" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="AC4" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AD4" s="49" t="s">
         <v>210</v>
@@ -2791,7 +2794,7 @@
         <v>216</v>
       </c>
       <c r="AI4" s="29" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AJ4" s="7" t="s">
         <v>165</v>
@@ -2812,7 +2815,7 @@
         <v>216</v>
       </c>
       <c r="AP4" s="29" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="AQ4" s="7" t="s">
         <v>168</v>
@@ -2878,20 +2881,20 @@
         <v>158</v>
       </c>
       <c r="BL4" s="46" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BM4" s="46" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="BN4" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="BO4" s="85" t="s">
+      <c r="BO4" s="93" t="s">
         <v>171</v>
       </c>
-      <c r="BP4" s="86"/>
-      <c r="BQ4" s="86"/>
-      <c r="BR4" s="86"/>
+      <c r="BP4" s="94"/>
+      <c r="BQ4" s="94"/>
+      <c r="BR4" s="94"/>
       <c r="BS4" s="5" t="s">
         <v>153</v>
       </c>
@@ -2907,10 +2910,10 @@
       <c r="BW4" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="BX4" s="57" t="s">
+      <c r="BX4" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="BY4" s="69"/>
+      <c r="BY4" s="75"/>
       <c r="BZ4" s="5" t="s">
         <v>175</v>
       </c>
@@ -2929,20 +2932,20 @@
       <c r="CE4" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="CF4" s="57" t="s">
+      <c r="CF4" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="CG4" s="69"/>
+      <c r="CG4" s="75"/>
       <c r="CH4" s="6" t="s">
         <v>178</v>
       </c>
       <c r="CI4" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="CJ4" s="57" t="s">
+      <c r="CJ4" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="CK4" s="69"/>
+      <c r="CK4" s="75"/>
       <c r="CL4" s="5" t="s">
         <v>153</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>152</v>
       </c>
       <c r="CP4" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="CQ4" s="5" t="s">
         <v>151</v>
@@ -2965,7 +2968,7 @@
         <v>152</v>
       </c>
       <c r="CS4" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="CT4" s="5" t="s">
         <v>153</v>
@@ -3003,21 +3006,21 @@
       <c r="DE4" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="DF4" s="57" t="s">
+      <c r="DF4" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="DG4" s="69"/>
-      <c r="DH4" s="57" t="s">
+      <c r="DG4" s="75"/>
+      <c r="DH4" s="74" t="s">
         <v>184</v>
       </c>
-      <c r="DI4" s="69"/>
+      <c r="DI4" s="75"/>
       <c r="DJ4" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="DK4" s="57" t="s">
+      <c r="DK4" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="DL4" s="69"/>
+      <c r="DL4" s="75"/>
       <c r="DM4" s="5" t="s">
         <v>182</v>
       </c>
@@ -3080,11 +3083,11 @@
       <c r="D5" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="89" t="s">
+      <c r="E5" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
       <c r="H5" s="28" t="s">
         <v>188</v>
       </c>
@@ -3103,10 +3106,10 @@
       <c r="M5" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="N5" s="93" t="s">
+      <c r="N5" s="72" t="s">
         <v>227</v>
       </c>
-      <c r="O5" s="94"/>
+      <c r="O5" s="81"/>
       <c r="P5" s="31" t="s">
         <v>187</v>
       </c>
@@ -3119,11 +3122,11 @@
       <c r="S5" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="T5" s="89" t="s">
+      <c r="T5" s="87" t="s">
         <v>187</v>
       </c>
-      <c r="U5" s="90"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="73"/>
       <c r="W5" s="42" t="s">
         <v>237</v>
       </c>
@@ -3139,24 +3142,24 @@
       <c r="AA5" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AB5" s="93" t="s">
+      <c r="AB5" s="72" t="s">
         <v>239</v>
       </c>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="57" t="s">
+      <c r="AC5" s="73"/>
+      <c r="AD5" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="57" t="s">
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="AG5" s="75"/>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="57" t="s">
+      <c r="AG5" s="97"/>
+      <c r="AH5" s="97"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="74" t="s">
         <v>190</v>
       </c>
-      <c r="AK5" s="69"/>
+      <c r="AK5" s="75"/>
       <c r="AL5" s="40" t="s">
         <v>231</v>
       </c>
@@ -3166,10 +3169,10 @@
       <c r="AN5" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="AO5" s="57" t="s">
+      <c r="AO5" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="AP5" s="69"/>
+      <c r="AP5" s="75"/>
       <c r="AQ5" s="5" t="s">
         <v>235</v>
       </c>
@@ -3179,49 +3182,49 @@
       <c r="AS5" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="AT5" s="60" t="s">
+      <c r="AT5" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="AU5" s="61"/>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="62"/>
-      <c r="AX5" s="60" t="s">
+      <c r="AU5" s="123"/>
+      <c r="AV5" s="123"/>
+      <c r="AW5" s="124"/>
+      <c r="AX5" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="61"/>
-      <c r="BA5" s="62"/>
-      <c r="BB5" s="60" t="s">
+      <c r="AY5" s="123"/>
+      <c r="AZ5" s="123"/>
+      <c r="BA5" s="124"/>
+      <c r="BB5" s="114" t="s">
         <v>242</v>
       </c>
-      <c r="BC5" s="61"/>
-      <c r="BD5" s="61"/>
-      <c r="BE5" s="62"/>
-      <c r="BF5" s="60" t="s">
+      <c r="BC5" s="123"/>
+      <c r="BD5" s="123"/>
+      <c r="BE5" s="124"/>
+      <c r="BF5" s="114" t="s">
         <v>243</v>
       </c>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="61"/>
-      <c r="BI5" s="62"/>
+      <c r="BG5" s="123"/>
+      <c r="BH5" s="123"/>
+      <c r="BI5" s="124"/>
       <c r="BJ5" s="31" t="s">
         <v>187</v>
       </c>
       <c r="BK5" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="BL5" s="87" t="s">
+      <c r="BL5" s="95" t="s">
         <v>245</v>
       </c>
-      <c r="BM5" s="88"/>
+      <c r="BM5" s="96"/>
       <c r="BN5" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="BO5" s="89" t="s">
+      <c r="BO5" s="87" t="s">
         <v>188</v>
       </c>
-      <c r="BP5" s="90"/>
-      <c r="BQ5" s="90"/>
-      <c r="BR5" s="91"/>
+      <c r="BP5" s="88"/>
+      <c r="BQ5" s="88"/>
+      <c r="BR5" s="73"/>
       <c r="BS5" s="14" t="s">
         <v>236</v>
       </c>
@@ -3234,11 +3237,11 @@
       <c r="BV5" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="BW5" s="57" t="s">
+      <c r="BW5" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="BX5" s="75"/>
-      <c r="BY5" s="75"/>
+      <c r="BX5" s="97"/>
+      <c r="BY5" s="97"/>
       <c r="BZ5" s="5" t="s">
         <v>187</v>
       </c>
@@ -3251,72 +3254,72 @@
       <c r="CC5" s="40" t="s">
         <v>249</v>
       </c>
-      <c r="CD5" s="57" t="s">
+      <c r="CD5" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="CE5" s="75"/>
-      <c r="CF5" s="75"/>
+      <c r="CE5" s="97"/>
+      <c r="CF5" s="97"/>
       <c r="CG5" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="CH5" s="57" t="s">
+      <c r="CH5" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="CI5" s="75"/>
-      <c r="CJ5" s="57" t="s">
+      <c r="CI5" s="97"/>
+      <c r="CJ5" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="CK5" s="75"/>
-      <c r="CL5" s="69"/>
+      <c r="CK5" s="97"/>
+      <c r="CL5" s="75"/>
       <c r="CM5" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="CN5" s="57" t="s">
+      <c r="CN5" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="CO5" s="75"/>
-      <c r="CP5" s="75"/>
-      <c r="CQ5" s="75"/>
-      <c r="CR5" s="75"/>
-      <c r="CS5" s="75"/>
+      <c r="CO5" s="97"/>
+      <c r="CP5" s="97"/>
+      <c r="CQ5" s="97"/>
+      <c r="CR5" s="97"/>
+      <c r="CS5" s="97"/>
       <c r="CT5" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="CU5" s="76" t="s">
+      <c r="CU5" s="111" t="s">
         <v>255</v>
       </c>
-      <c r="CV5" s="77"/>
-      <c r="CW5" s="78"/>
-      <c r="CX5" s="57" t="s">
+      <c r="CV5" s="112"/>
+      <c r="CW5" s="113"/>
+      <c r="CX5" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="CY5" s="75"/>
-      <c r="CZ5" s="75"/>
-      <c r="DA5" s="57" t="s">
+      <c r="CY5" s="97"/>
+      <c r="CZ5" s="97"/>
+      <c r="DA5" s="74" t="s">
+        <v>268</v>
+      </c>
+      <c r="DB5" s="75"/>
+      <c r="DC5" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="DD5" s="82" t="s">
+        <v>268</v>
+      </c>
+      <c r="DE5" s="75"/>
+      <c r="DF5" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="DG5" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="DB5" s="69"/>
-      <c r="DC5" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="DD5" s="66" t="s">
-        <v>256</v>
-      </c>
-      <c r="DE5" s="69"/>
-      <c r="DF5" s="10" t="s">
+      <c r="DH5" s="82" t="s">
         <v>225</v>
       </c>
-      <c r="DG5" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="DH5" s="66" t="s">
-        <v>225</v>
-      </c>
-      <c r="DI5" s="69"/>
-      <c r="DJ5" s="57" t="s">
+      <c r="DI5" s="75"/>
+      <c r="DJ5" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="DK5" s="69"/>
+      <c r="DK5" s="75"/>
       <c r="DL5" s="5" t="s">
         <v>228</v>
       </c>
@@ -3326,48 +3329,48 @@
       <c r="DN5" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="DO5" s="60" t="s">
+      <c r="DO5" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="DP5" s="75"/>
+      <c r="DQ5" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="DR5" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="DS5" s="75"/>
+      <c r="DT5" s="115" t="s">
+        <v>226</v>
+      </c>
+      <c r="DU5" s="75"/>
+      <c r="DV5" s="74" t="s">
+        <v>227</v>
+      </c>
+      <c r="DW5" s="97"/>
+      <c r="DX5" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="DP5" s="69"/>
-      <c r="DQ5" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="DR5" s="60" t="s">
+      <c r="DY5" s="114" t="s">
         <v>259</v>
       </c>
-      <c r="DS5" s="69"/>
-      <c r="DT5" s="58" t="s">
-        <v>226</v>
-      </c>
-      <c r="DU5" s="69"/>
-      <c r="DV5" s="57" t="s">
+      <c r="DZ5" s="97"/>
+      <c r="EA5" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="DW5" s="75"/>
-      <c r="DX5" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="DY5" s="60" t="s">
-        <v>261</v>
-      </c>
-      <c r="DZ5" s="75"/>
-      <c r="EA5" s="57" t="s">
-        <v>227</v>
-      </c>
-      <c r="EB5" s="69"/>
+      <c r="EB5" s="75"/>
     </row>
     <row r="6" spans="1:132" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="67"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
       <c r="I6" s="34"/>
       <c r="J6" s="31" t="s">
         <v>192</v>
@@ -3375,145 +3378,145 @@
       <c r="K6" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="L6" s="95" t="s">
+      <c r="L6" s="76" t="s">
         <v>224</v>
       </c>
-      <c r="M6" s="96"/>
-      <c r="N6" s="96"/>
-      <c r="O6" s="97"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="78"/>
       <c r="P6" s="35"/>
       <c r="Q6" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="R6" s="99"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="68"/>
-      <c r="Z6" s="68"/>
-      <c r="AA6" s="68"/>
-      <c r="AB6" s="68"/>
-      <c r="AC6" s="68"/>
-      <c r="AD6" s="68"/>
-      <c r="AE6" s="67"/>
-      <c r="AF6" s="66"/>
-      <c r="AG6" s="68"/>
-      <c r="AH6" s="68"/>
-      <c r="AI6" s="68"/>
-      <c r="AJ6" s="68"/>
-      <c r="AK6" s="68"/>
-      <c r="AL6" s="68"/>
-      <c r="AM6" s="68"/>
-      <c r="AN6" s="67"/>
-      <c r="AO6" s="70" t="s">
+      <c r="R6" s="85"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
+      <c r="Z6" s="83"/>
+      <c r="AA6" s="83"/>
+      <c r="AB6" s="83"/>
+      <c r="AC6" s="83"/>
+      <c r="AD6" s="83"/>
+      <c r="AE6" s="84"/>
+      <c r="AF6" s="82"/>
+      <c r="AG6" s="83"/>
+      <c r="AH6" s="83"/>
+      <c r="AI6" s="83"/>
+      <c r="AJ6" s="83"/>
+      <c r="AK6" s="83"/>
+      <c r="AL6" s="83"/>
+      <c r="AM6" s="83"/>
+      <c r="AN6" s="84"/>
+      <c r="AO6" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="AP6" s="71"/>
+      <c r="AP6" s="116"/>
       <c r="AQ6" s="11"/>
       <c r="AR6" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="AS6" s="66"/>
-      <c r="AT6" s="68"/>
-      <c r="AU6" s="68"/>
-      <c r="AV6" s="68"/>
-      <c r="AW6" s="68"/>
-      <c r="AX6" s="68"/>
-      <c r="AY6" s="68"/>
-      <c r="AZ6" s="68"/>
-      <c r="BA6" s="68"/>
-      <c r="BB6" s="68"/>
-      <c r="BC6" s="68"/>
-      <c r="BD6" s="68"/>
-      <c r="BE6" s="68"/>
-      <c r="BF6" s="68"/>
-      <c r="BG6" s="68"/>
-      <c r="BH6" s="68"/>
-      <c r="BI6" s="67"/>
-      <c r="BJ6" s="66"/>
-      <c r="BK6" s="68"/>
-      <c r="BL6" s="68"/>
-      <c r="BM6" s="68"/>
-      <c r="BN6" s="68"/>
-      <c r="BO6" s="68"/>
-      <c r="BP6" s="68"/>
-      <c r="BQ6" s="68"/>
-      <c r="BR6" s="67"/>
-      <c r="BS6" s="70" t="s">
+      <c r="AS6" s="82"/>
+      <c r="AT6" s="83"/>
+      <c r="AU6" s="83"/>
+      <c r="AV6" s="83"/>
+      <c r="AW6" s="83"/>
+      <c r="AX6" s="83"/>
+      <c r="AY6" s="83"/>
+      <c r="AZ6" s="83"/>
+      <c r="BA6" s="83"/>
+      <c r="BB6" s="83"/>
+      <c r="BC6" s="83"/>
+      <c r="BD6" s="83"/>
+      <c r="BE6" s="83"/>
+      <c r="BF6" s="83"/>
+      <c r="BG6" s="83"/>
+      <c r="BH6" s="83"/>
+      <c r="BI6" s="84"/>
+      <c r="BJ6" s="82"/>
+      <c r="BK6" s="83"/>
+      <c r="BL6" s="83"/>
+      <c r="BM6" s="83"/>
+      <c r="BN6" s="83"/>
+      <c r="BO6" s="83"/>
+      <c r="BP6" s="83"/>
+      <c r="BQ6" s="83"/>
+      <c r="BR6" s="84"/>
+      <c r="BS6" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="BT6" s="84"/>
-      <c r="BU6" s="66"/>
-      <c r="BV6" s="68"/>
-      <c r="BW6" s="68"/>
-      <c r="BX6" s="68"/>
-      <c r="BY6" s="67"/>
-      <c r="BZ6" s="66"/>
-      <c r="CA6" s="67"/>
-      <c r="CB6" s="70" t="s">
+      <c r="BT6" s="100"/>
+      <c r="BU6" s="82"/>
+      <c r="BV6" s="83"/>
+      <c r="BW6" s="83"/>
+      <c r="BX6" s="83"/>
+      <c r="BY6" s="84"/>
+      <c r="BZ6" s="82"/>
+      <c r="CA6" s="84"/>
+      <c r="CB6" s="99" t="s">
         <v>194</v>
       </c>
-      <c r="CC6" s="84"/>
-      <c r="CD6" s="66"/>
-      <c r="CE6" s="68"/>
-      <c r="CF6" s="67"/>
-      <c r="CG6" s="66" t="s">
+      <c r="CC6" s="100"/>
+      <c r="CD6" s="82"/>
+      <c r="CE6" s="83"/>
+      <c r="CF6" s="84"/>
+      <c r="CG6" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="CH6" s="73"/>
-      <c r="CI6" s="73"/>
-      <c r="CJ6" s="73"/>
-      <c r="CK6" s="73"/>
-      <c r="CL6" s="73"/>
-      <c r="CM6" s="73"/>
-      <c r="CN6" s="73"/>
-      <c r="CO6" s="73"/>
-      <c r="CP6" s="73"/>
-      <c r="CQ6" s="73"/>
-      <c r="CR6" s="73"/>
-      <c r="CS6" s="73"/>
-      <c r="CT6" s="73"/>
-      <c r="CU6" s="73"/>
-      <c r="CV6" s="73"/>
-      <c r="CW6" s="73"/>
-      <c r="CX6" s="73"/>
-      <c r="CY6" s="73"/>
-      <c r="CZ6" s="73"/>
-      <c r="DA6" s="73"/>
-      <c r="DB6" s="73"/>
-      <c r="DC6" s="73"/>
-      <c r="DD6" s="73"/>
-      <c r="DE6" s="73"/>
-      <c r="DF6" s="73"/>
-      <c r="DG6" s="73"/>
-      <c r="DH6" s="73"/>
-      <c r="DI6" s="74"/>
-      <c r="DJ6" s="70" t="s">
+      <c r="CH6" s="89"/>
+      <c r="CI6" s="89"/>
+      <c r="CJ6" s="89"/>
+      <c r="CK6" s="89"/>
+      <c r="CL6" s="89"/>
+      <c r="CM6" s="89"/>
+      <c r="CN6" s="89"/>
+      <c r="CO6" s="89"/>
+      <c r="CP6" s="89"/>
+      <c r="CQ6" s="89"/>
+      <c r="CR6" s="89"/>
+      <c r="CS6" s="89"/>
+      <c r="CT6" s="89"/>
+      <c r="CU6" s="89"/>
+      <c r="CV6" s="89"/>
+      <c r="CW6" s="89"/>
+      <c r="CX6" s="89"/>
+      <c r="CY6" s="89"/>
+      <c r="CZ6" s="89"/>
+      <c r="DA6" s="89"/>
+      <c r="DB6" s="89"/>
+      <c r="DC6" s="89"/>
+      <c r="DD6" s="89"/>
+      <c r="DE6" s="89"/>
+      <c r="DF6" s="89"/>
+      <c r="DG6" s="89"/>
+      <c r="DH6" s="89"/>
+      <c r="DI6" s="79"/>
+      <c r="DJ6" s="99" t="s">
         <v>193</v>
       </c>
-      <c r="DK6" s="71"/>
-      <c r="DL6" s="71"/>
-      <c r="DM6" s="71"/>
-      <c r="DN6" s="71"/>
-      <c r="DO6" s="71"/>
-      <c r="DP6" s="71"/>
-      <c r="DQ6" s="71"/>
-      <c r="DR6" s="71"/>
-      <c r="DS6" s="71"/>
-      <c r="DT6" s="71"/>
-      <c r="DU6" s="71"/>
-      <c r="DV6" s="72" t="s">
+      <c r="DK6" s="116"/>
+      <c r="DL6" s="116"/>
+      <c r="DM6" s="116"/>
+      <c r="DN6" s="116"/>
+      <c r="DO6" s="116"/>
+      <c r="DP6" s="116"/>
+      <c r="DQ6" s="116"/>
+      <c r="DR6" s="116"/>
+      <c r="DS6" s="116"/>
+      <c r="DT6" s="116"/>
+      <c r="DU6" s="116"/>
+      <c r="DV6" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="DW6" s="73"/>
-      <c r="DX6" s="73"/>
-      <c r="DY6" s="73"/>
-      <c r="DZ6" s="73"/>
-      <c r="EA6" s="73"/>
-      <c r="EB6" s="74"/>
+      <c r="DW6" s="89"/>
+      <c r="DX6" s="89"/>
+      <c r="DY6" s="89"/>
+      <c r="DZ6" s="89"/>
+      <c r="EA6" s="89"/>
+      <c r="EB6" s="79"/>
     </row>
     <row r="7" spans="1:132" ht="23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -3526,575 +3529,575 @@
         <v>188</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="74" t="s">
         <v>188</v>
       </c>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="79"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="65"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="59"/>
-      <c r="AB7" s="57" t="s">
+      <c r="I7" s="117"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="119"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="115"/>
+      <c r="V7" s="115"/>
+      <c r="W7" s="115"/>
+      <c r="X7" s="115"/>
+      <c r="Y7" s="115"/>
+      <c r="Z7" s="115"/>
+      <c r="AA7" s="120"/>
+      <c r="AB7" s="74" t="s">
         <v>188</v>
       </c>
-      <c r="AC7" s="74"/>
-      <c r="AD7" s="57"/>
-      <c r="AE7" s="59"/>
-      <c r="AF7" s="92" t="s">
+      <c r="AC7" s="79"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="120"/>
+      <c r="AF7" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="AG7" s="84"/>
-      <c r="AH7" s="57"/>
-      <c r="AI7" s="59"/>
+      <c r="AG7" s="100"/>
+      <c r="AH7" s="74"/>
+      <c r="AI7" s="120"/>
       <c r="AJ7" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="AK7" s="57"/>
-      <c r="AL7" s="58"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="58"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="58"/>
-      <c r="AW7" s="58"/>
-      <c r="AX7" s="58"/>
-      <c r="AY7" s="58"/>
-      <c r="AZ7" s="58"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="58"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="58"/>
-      <c r="BE7" s="58"/>
-      <c r="BF7" s="58"/>
-      <c r="BG7" s="58"/>
-      <c r="BH7" s="58"/>
-      <c r="BI7" s="59"/>
-      <c r="BJ7" s="57"/>
-      <c r="BK7" s="58"/>
-      <c r="BL7" s="58"/>
-      <c r="BM7" s="58"/>
-      <c r="BN7" s="58"/>
-      <c r="BO7" s="58"/>
-      <c r="BP7" s="58"/>
-      <c r="BQ7" s="58"/>
-      <c r="BR7" s="58"/>
-      <c r="BS7" s="58"/>
-      <c r="BT7" s="59"/>
-      <c r="BU7" s="57"/>
-      <c r="BV7" s="58"/>
-      <c r="BW7" s="58"/>
-      <c r="BX7" s="58"/>
-      <c r="BY7" s="59"/>
-      <c r="BZ7" s="57"/>
-      <c r="CA7" s="58"/>
-      <c r="CB7" s="58"/>
-      <c r="CC7" s="58"/>
-      <c r="CD7" s="58"/>
-      <c r="CE7" s="58"/>
-      <c r="CF7" s="58"/>
-      <c r="CG7" s="59"/>
-      <c r="CH7" s="57"/>
-      <c r="CI7" s="58"/>
-      <c r="CJ7" s="58"/>
-      <c r="CK7" s="58"/>
-      <c r="CL7" s="58"/>
-      <c r="CM7" s="58"/>
-      <c r="CN7" s="58"/>
-      <c r="CO7" s="58"/>
-      <c r="CP7" s="58"/>
-      <c r="CQ7" s="58"/>
-      <c r="CR7" s="58"/>
-      <c r="CS7" s="58"/>
-      <c r="CT7" s="58"/>
-      <c r="CU7" s="58"/>
-      <c r="CV7" s="58"/>
-      <c r="CW7" s="58"/>
-      <c r="CX7" s="58"/>
-      <c r="CY7" s="58"/>
-      <c r="CZ7" s="58"/>
-      <c r="DA7" s="58"/>
-      <c r="DB7" s="58"/>
-      <c r="DC7" s="58"/>
-      <c r="DD7" s="58"/>
-      <c r="DE7" s="58"/>
-      <c r="DF7" s="58"/>
-      <c r="DG7" s="58"/>
-      <c r="DH7" s="58"/>
-      <c r="DI7" s="59"/>
-      <c r="DJ7" s="57"/>
-      <c r="DK7" s="58"/>
-      <c r="DL7" s="58"/>
-      <c r="DM7" s="58"/>
-      <c r="DN7" s="58"/>
-      <c r="DO7" s="58"/>
-      <c r="DP7" s="58"/>
-      <c r="DQ7" s="58"/>
-      <c r="DR7" s="58"/>
-      <c r="DS7" s="58"/>
-      <c r="DT7" s="58"/>
-      <c r="DU7" s="59"/>
-      <c r="DV7" s="57"/>
-      <c r="DW7" s="58"/>
-      <c r="DX7" s="58"/>
-      <c r="DY7" s="58"/>
-      <c r="DZ7" s="58"/>
-      <c r="EA7" s="58"/>
-      <c r="EB7" s="59"/>
+      <c r="AK7" s="74"/>
+      <c r="AL7" s="115"/>
+      <c r="AM7" s="115"/>
+      <c r="AN7" s="115"/>
+      <c r="AO7" s="115"/>
+      <c r="AP7" s="115"/>
+      <c r="AQ7" s="115"/>
+      <c r="AR7" s="115"/>
+      <c r="AS7" s="115"/>
+      <c r="AT7" s="115"/>
+      <c r="AU7" s="115"/>
+      <c r="AV7" s="115"/>
+      <c r="AW7" s="115"/>
+      <c r="AX7" s="115"/>
+      <c r="AY7" s="115"/>
+      <c r="AZ7" s="115"/>
+      <c r="BA7" s="115"/>
+      <c r="BB7" s="115"/>
+      <c r="BC7" s="115"/>
+      <c r="BD7" s="115"/>
+      <c r="BE7" s="115"/>
+      <c r="BF7" s="115"/>
+      <c r="BG7" s="115"/>
+      <c r="BH7" s="115"/>
+      <c r="BI7" s="120"/>
+      <c r="BJ7" s="74"/>
+      <c r="BK7" s="115"/>
+      <c r="BL7" s="115"/>
+      <c r="BM7" s="115"/>
+      <c r="BN7" s="115"/>
+      <c r="BO7" s="115"/>
+      <c r="BP7" s="115"/>
+      <c r="BQ7" s="115"/>
+      <c r="BR7" s="115"/>
+      <c r="BS7" s="115"/>
+      <c r="BT7" s="120"/>
+      <c r="BU7" s="74"/>
+      <c r="BV7" s="115"/>
+      <c r="BW7" s="115"/>
+      <c r="BX7" s="115"/>
+      <c r="BY7" s="120"/>
+      <c r="BZ7" s="74"/>
+      <c r="CA7" s="115"/>
+      <c r="CB7" s="115"/>
+      <c r="CC7" s="115"/>
+      <c r="CD7" s="115"/>
+      <c r="CE7" s="115"/>
+      <c r="CF7" s="115"/>
+      <c r="CG7" s="120"/>
+      <c r="CH7" s="74"/>
+      <c r="CI7" s="115"/>
+      <c r="CJ7" s="115"/>
+      <c r="CK7" s="115"/>
+      <c r="CL7" s="115"/>
+      <c r="CM7" s="115"/>
+      <c r="CN7" s="115"/>
+      <c r="CO7" s="115"/>
+      <c r="CP7" s="115"/>
+      <c r="CQ7" s="115"/>
+      <c r="CR7" s="115"/>
+      <c r="CS7" s="115"/>
+      <c r="CT7" s="115"/>
+      <c r="CU7" s="115"/>
+      <c r="CV7" s="115"/>
+      <c r="CW7" s="115"/>
+      <c r="CX7" s="115"/>
+      <c r="CY7" s="115"/>
+      <c r="CZ7" s="115"/>
+      <c r="DA7" s="115"/>
+      <c r="DB7" s="115"/>
+      <c r="DC7" s="115"/>
+      <c r="DD7" s="115"/>
+      <c r="DE7" s="115"/>
+      <c r="DF7" s="115"/>
+      <c r="DG7" s="115"/>
+      <c r="DH7" s="115"/>
+      <c r="DI7" s="120"/>
+      <c r="DJ7" s="74"/>
+      <c r="DK7" s="115"/>
+      <c r="DL7" s="115"/>
+      <c r="DM7" s="115"/>
+      <c r="DN7" s="115"/>
+      <c r="DO7" s="115"/>
+      <c r="DP7" s="115"/>
+      <c r="DQ7" s="115"/>
+      <c r="DR7" s="115"/>
+      <c r="DS7" s="115"/>
+      <c r="DT7" s="115"/>
+      <c r="DU7" s="120"/>
+      <c r="DV7" s="74"/>
+      <c r="DW7" s="115"/>
+      <c r="DX7" s="115"/>
+      <c r="DY7" s="115"/>
+      <c r="DZ7" s="115"/>
+      <c r="EA7" s="115"/>
+      <c r="EB7" s="120"/>
     </row>
     <row r="8" spans="1:132" s="39" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B8" s="124">
+        <v>267</v>
+      </c>
+      <c r="B8" s="71">
         <v>1</v>
       </c>
-      <c r="C8" s="124">
+      <c r="C8" s="71">
         <v>2</v>
       </c>
-      <c r="D8" s="124">
+      <c r="D8" s="71">
         <v>3</v>
       </c>
-      <c r="E8" s="124">
+      <c r="E8" s="71">
         <v>4</v>
       </c>
-      <c r="F8" s="124">
+      <c r="F8" s="71">
         <v>5</v>
       </c>
-      <c r="G8" s="124">
+      <c r="G8" s="71">
         <v>6</v>
       </c>
-      <c r="H8" s="124">
+      <c r="H8" s="71">
         <v>7</v>
       </c>
-      <c r="I8" s="124">
+      <c r="I8" s="71">
         <v>8</v>
       </c>
-      <c r="J8" s="124">
+      <c r="J8" s="71">
         <v>9</v>
       </c>
-      <c r="K8" s="124">
+      <c r="K8" s="71">
         <v>10</v>
       </c>
-      <c r="L8" s="124">
+      <c r="L8" s="71">
         <v>11</v>
       </c>
-      <c r="M8" s="124">
+      <c r="M8" s="71">
         <v>12</v>
       </c>
-      <c r="N8" s="124">
+      <c r="N8" s="71">
         <v>13</v>
       </c>
-      <c r="O8" s="124">
+      <c r="O8" s="71">
         <v>14</v>
       </c>
-      <c r="P8" s="124">
+      <c r="P8" s="71">
         <v>15</v>
       </c>
-      <c r="Q8" s="124">
+      <c r="Q8" s="71">
         <v>16</v>
       </c>
-      <c r="R8" s="124">
+      <c r="R8" s="71">
         <v>17</v>
       </c>
-      <c r="S8" s="124">
+      <c r="S8" s="71">
         <v>18</v>
       </c>
-      <c r="T8" s="124">
+      <c r="T8" s="71">
         <v>19</v>
       </c>
-      <c r="U8" s="124">
+      <c r="U8" s="71">
         <v>20</v>
       </c>
-      <c r="V8" s="124">
+      <c r="V8" s="71">
         <v>21</v>
       </c>
-      <c r="W8" s="124">
+      <c r="W8" s="71">
         <v>22</v>
       </c>
-      <c r="X8" s="124">
+      <c r="X8" s="71">
         <v>23</v>
       </c>
-      <c r="Y8" s="124">
+      <c r="Y8" s="71">
         <v>24</v>
       </c>
-      <c r="Z8" s="124">
+      <c r="Z8" s="71">
         <v>25</v>
       </c>
-      <c r="AA8" s="124">
+      <c r="AA8" s="71">
         <v>26</v>
       </c>
-      <c r="AB8" s="124">
+      <c r="AB8" s="71">
         <v>27</v>
       </c>
-      <c r="AC8" s="124">
+      <c r="AC8" s="71">
         <v>28</v>
       </c>
-      <c r="AD8" s="124">
+      <c r="AD8" s="71">
         <v>29</v>
       </c>
-      <c r="AE8" s="124">
+      <c r="AE8" s="71">
         <v>30</v>
       </c>
-      <c r="AF8" s="124">
+      <c r="AF8" s="71">
         <v>31</v>
       </c>
-      <c r="AG8" s="124">
+      <c r="AG8" s="71">
         <v>32</v>
       </c>
-      <c r="AH8" s="124">
+      <c r="AH8" s="71">
         <v>33</v>
       </c>
-      <c r="AI8" s="124">
+      <c r="AI8" s="71">
         <v>34</v>
       </c>
-      <c r="AJ8" s="124">
+      <c r="AJ8" s="71">
         <v>35</v>
       </c>
-      <c r="AK8" s="124">
+      <c r="AK8" s="71">
         <v>36</v>
       </c>
-      <c r="AL8" s="124">
+      <c r="AL8" s="71">
         <v>37</v>
       </c>
-      <c r="AM8" s="124">
+      <c r="AM8" s="71">
         <v>38</v>
       </c>
-      <c r="AN8" s="124">
+      <c r="AN8" s="71">
         <v>39</v>
       </c>
-      <c r="AO8" s="124">
+      <c r="AO8" s="71">
         <v>40</v>
       </c>
-      <c r="AP8" s="124">
+      <c r="AP8" s="71">
         <v>41</v>
       </c>
-      <c r="AQ8" s="124">
+      <c r="AQ8" s="71">
         <v>42</v>
       </c>
-      <c r="AR8" s="124">
+      <c r="AR8" s="71">
         <v>43</v>
       </c>
-      <c r="AS8" s="124">
+      <c r="AS8" s="71">
         <v>44</v>
       </c>
-      <c r="AT8" s="124">
+      <c r="AT8" s="71">
         <v>45</v>
       </c>
-      <c r="AU8" s="124">
+      <c r="AU8" s="71">
         <v>46</v>
       </c>
-      <c r="AV8" s="124">
+      <c r="AV8" s="71">
         <v>47</v>
       </c>
-      <c r="AW8" s="124">
+      <c r="AW8" s="71">
         <v>48</v>
       </c>
-      <c r="AX8" s="124">
+      <c r="AX8" s="71">
         <v>49</v>
       </c>
-      <c r="AY8" s="124">
+      <c r="AY8" s="71">
         <v>50</v>
       </c>
-      <c r="AZ8" s="124">
+      <c r="AZ8" s="71">
         <v>51</v>
       </c>
-      <c r="BA8" s="124">
+      <c r="BA8" s="71">
         <v>52</v>
       </c>
-      <c r="BB8" s="124">
+      <c r="BB8" s="71">
         <v>53</v>
       </c>
-      <c r="BC8" s="124">
+      <c r="BC8" s="71">
         <v>54</v>
       </c>
-      <c r="BD8" s="124">
+      <c r="BD8" s="71">
         <v>55</v>
       </c>
-      <c r="BE8" s="124">
+      <c r="BE8" s="71">
         <v>56</v>
       </c>
-      <c r="BF8" s="124">
+      <c r="BF8" s="71">
         <v>57</v>
       </c>
-      <c r="BG8" s="124">
+      <c r="BG8" s="71">
         <v>58</v>
       </c>
-      <c r="BH8" s="124">
+      <c r="BH8" s="71">
         <v>59</v>
       </c>
-      <c r="BI8" s="124">
+      <c r="BI8" s="71">
         <v>60</v>
       </c>
-      <c r="BJ8" s="124">
+      <c r="BJ8" s="71">
         <v>61</v>
       </c>
-      <c r="BK8" s="124">
+      <c r="BK8" s="71">
         <v>62</v>
       </c>
-      <c r="BL8" s="124">
+      <c r="BL8" s="71">
         <v>63</v>
       </c>
-      <c r="BM8" s="124">
+      <c r="BM8" s="71">
         <v>64</v>
       </c>
-      <c r="BN8" s="124">
+      <c r="BN8" s="71">
         <v>65</v>
       </c>
-      <c r="BO8" s="124">
+      <c r="BO8" s="71">
         <v>66</v>
       </c>
-      <c r="BP8" s="124">
+      <c r="BP8" s="71">
         <v>67</v>
       </c>
-      <c r="BQ8" s="124">
+      <c r="BQ8" s="71">
         <v>68</v>
       </c>
-      <c r="BR8" s="124">
+      <c r="BR8" s="71">
         <v>69</v>
       </c>
-      <c r="BS8" s="124">
+      <c r="BS8" s="71">
         <v>70</v>
       </c>
-      <c r="BT8" s="124">
+      <c r="BT8" s="71">
         <v>71</v>
       </c>
-      <c r="BU8" s="124">
+      <c r="BU8" s="71">
         <v>72</v>
       </c>
-      <c r="BV8" s="124">
+      <c r="BV8" s="71">
         <v>73</v>
       </c>
-      <c r="BW8" s="124">
+      <c r="BW8" s="71">
         <v>74</v>
       </c>
-      <c r="BX8" s="124">
+      <c r="BX8" s="71">
         <v>75</v>
       </c>
-      <c r="BY8" s="124">
+      <c r="BY8" s="71">
         <v>76</v>
       </c>
-      <c r="BZ8" s="124">
+      <c r="BZ8" s="71">
         <v>77</v>
       </c>
-      <c r="CA8" s="124">
+      <c r="CA8" s="71">
         <v>78</v>
       </c>
-      <c r="CB8" s="124">
+      <c r="CB8" s="71">
         <v>79</v>
       </c>
-      <c r="CC8" s="124">
+      <c r="CC8" s="71">
         <v>80</v>
       </c>
-      <c r="CD8" s="124">
+      <c r="CD8" s="71">
         <v>81</v>
       </c>
-      <c r="CE8" s="124">
+      <c r="CE8" s="71">
         <v>82</v>
       </c>
-      <c r="CF8" s="124">
+      <c r="CF8" s="71">
         <v>83</v>
       </c>
-      <c r="CG8" s="124">
+      <c r="CG8" s="71">
         <v>84</v>
       </c>
-      <c r="CH8" s="124">
+      <c r="CH8" s="71">
         <v>85</v>
       </c>
-      <c r="CI8" s="124">
+      <c r="CI8" s="71">
         <v>86</v>
       </c>
-      <c r="CJ8" s="124">
+      <c r="CJ8" s="71">
         <v>87</v>
       </c>
-      <c r="CK8" s="124">
+      <c r="CK8" s="71">
         <v>88</v>
       </c>
-      <c r="CL8" s="124">
+      <c r="CL8" s="71">
         <v>89</v>
       </c>
-      <c r="CM8" s="124">
+      <c r="CM8" s="71">
         <v>90</v>
       </c>
-      <c r="CN8" s="124">
+      <c r="CN8" s="71">
         <v>91</v>
       </c>
-      <c r="CO8" s="124">
+      <c r="CO8" s="71">
         <v>92</v>
       </c>
-      <c r="CP8" s="124">
+      <c r="CP8" s="71">
         <v>93</v>
       </c>
-      <c r="CQ8" s="124">
+      <c r="CQ8" s="71">
         <v>94</v>
       </c>
-      <c r="CR8" s="124">
+      <c r="CR8" s="71">
         <v>95</v>
       </c>
-      <c r="CS8" s="124">
+      <c r="CS8" s="71">
         <v>96</v>
       </c>
-      <c r="CT8" s="124">
+      <c r="CT8" s="71">
         <v>97</v>
       </c>
-      <c r="CU8" s="124">
+      <c r="CU8" s="71">
         <v>98</v>
       </c>
-      <c r="CV8" s="124">
+      <c r="CV8" s="71">
         <v>99</v>
       </c>
-      <c r="CW8" s="124">
+      <c r="CW8" s="71">
         <v>100</v>
       </c>
-      <c r="CX8" s="124">
+      <c r="CX8" s="71">
         <v>101</v>
       </c>
-      <c r="CY8" s="124">
+      <c r="CY8" s="71">
         <v>102</v>
       </c>
-      <c r="CZ8" s="124">
+      <c r="CZ8" s="71">
         <v>103</v>
       </c>
-      <c r="DA8" s="124">
+      <c r="DA8" s="71">
         <v>104</v>
       </c>
-      <c r="DB8" s="124">
+      <c r="DB8" s="71">
         <v>105</v>
       </c>
-      <c r="DC8" s="124">
+      <c r="DC8" s="71">
         <v>106</v>
       </c>
-      <c r="DD8" s="124">
+      <c r="DD8" s="71">
         <v>107</v>
       </c>
-      <c r="DE8" s="124">
+      <c r="DE8" s="71">
         <v>108</v>
       </c>
-      <c r="DF8" s="124">
+      <c r="DF8" s="71">
         <v>109</v>
       </c>
-      <c r="DG8" s="124">
+      <c r="DG8" s="71">
         <v>110</v>
       </c>
-      <c r="DH8" s="124">
+      <c r="DH8" s="71">
         <v>111</v>
       </c>
-      <c r="DI8" s="124">
+      <c r="DI8" s="71">
         <v>112</v>
       </c>
-      <c r="DJ8" s="124">
+      <c r="DJ8" s="71">
         <v>113</v>
       </c>
-      <c r="DK8" s="124">
+      <c r="DK8" s="71">
         <v>114</v>
       </c>
-      <c r="DL8" s="124">
+      <c r="DL8" s="71">
         <v>115</v>
       </c>
-      <c r="DM8" s="124">
+      <c r="DM8" s="71">
         <v>116</v>
       </c>
-      <c r="DN8" s="124">
+      <c r="DN8" s="71">
         <v>117</v>
       </c>
-      <c r="DO8" s="124">
+      <c r="DO8" s="71">
         <v>118</v>
       </c>
-      <c r="DP8" s="124">
+      <c r="DP8" s="71">
         <v>119</v>
       </c>
-      <c r="DQ8" s="124">
+      <c r="DQ8" s="71">
         <v>120</v>
       </c>
-      <c r="DR8" s="124">
+      <c r="DR8" s="71">
         <v>121</v>
       </c>
-      <c r="DS8" s="124">
+      <c r="DS8" s="71">
         <v>122</v>
       </c>
-      <c r="DT8" s="124">
+      <c r="DT8" s="71">
         <v>123</v>
       </c>
-      <c r="DU8" s="124">
+      <c r="DU8" s="71">
         <v>124</v>
       </c>
-      <c r="DV8" s="124">
+      <c r="DV8" s="71">
         <v>125</v>
       </c>
-      <c r="DW8" s="124">
+      <c r="DW8" s="71">
         <v>126</v>
       </c>
-      <c r="DX8" s="124">
+      <c r="DX8" s="71">
         <v>127</v>
       </c>
-      <c r="DY8" s="124">
+      <c r="DY8" s="71">
         <v>128</v>
       </c>
-      <c r="DZ8" s="124">
+      <c r="DZ8" s="71">
         <v>129</v>
       </c>
-      <c r="EA8" s="124">
+      <c r="EA8" s="71">
         <v>130</v>
       </c>
-      <c r="EB8" s="124">
+      <c r="EB8" s="71">
         <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="L6:O6"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="T6:AE6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="CQ3:CS3"/>
-    <mergeCell ref="BO4:BR4"/>
-    <mergeCell ref="BX4:BY4"/>
-    <mergeCell ref="BL5:BM5"/>
-    <mergeCell ref="BO5:BR5"/>
-    <mergeCell ref="BW5:BY5"/>
-    <mergeCell ref="CH5:CI5"/>
-    <mergeCell ref="CD5:CF5"/>
-    <mergeCell ref="BZ1:CG1"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="CB6:CC6"/>
-    <mergeCell ref="BK3:BN3"/>
-    <mergeCell ref="CN3:CP3"/>
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="T1:AE1"/>
-    <mergeCell ref="AF1:BI1"/>
-    <mergeCell ref="BJ1:BT1"/>
-    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="DV1:EB1"/>
+    <mergeCell ref="DV7:EB7"/>
+    <mergeCell ref="AT5:AW5"/>
+    <mergeCell ref="AX5:BA5"/>
+    <mergeCell ref="BB5:BE5"/>
+    <mergeCell ref="BF5:BI5"/>
+    <mergeCell ref="BJ7:BT7"/>
+    <mergeCell ref="BU7:BY7"/>
+    <mergeCell ref="BZ7:CG7"/>
+    <mergeCell ref="CH7:DI7"/>
+    <mergeCell ref="DJ7:DU7"/>
+    <mergeCell ref="BZ6:CA6"/>
+    <mergeCell ref="BU6:BY6"/>
+    <mergeCell ref="BJ6:BR6"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AK7:BI7"/>
+    <mergeCell ref="AF7:AG7"/>
+    <mergeCell ref="CH1:DI1"/>
+    <mergeCell ref="DJ1:DU1"/>
+    <mergeCell ref="AS6:BI6"/>
+    <mergeCell ref="AF6:AN6"/>
+    <mergeCell ref="DO5:DP5"/>
+    <mergeCell ref="DR5:DS5"/>
+    <mergeCell ref="CD6:CF6"/>
+    <mergeCell ref="DJ6:DU6"/>
+    <mergeCell ref="AF5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="DD5:DE5"/>
+    <mergeCell ref="DH5:DI5"/>
+    <mergeCell ref="DJ5:DK5"/>
+    <mergeCell ref="AO6:AP6"/>
     <mergeCell ref="DV6:EB6"/>
     <mergeCell ref="CF4:CG4"/>
     <mergeCell ref="CJ4:CK4"/>
@@ -4111,41 +4114,41 @@
     <mergeCell ref="DK4:DL4"/>
     <mergeCell ref="CX5:CZ5"/>
     <mergeCell ref="DA5:DB5"/>
-    <mergeCell ref="AS6:BI6"/>
-    <mergeCell ref="AF6:AN6"/>
-    <mergeCell ref="DO5:DP5"/>
-    <mergeCell ref="DR5:DS5"/>
-    <mergeCell ref="CD6:CF6"/>
-    <mergeCell ref="DJ6:DU6"/>
-    <mergeCell ref="AF5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="DD5:DE5"/>
-    <mergeCell ref="DH5:DI5"/>
-    <mergeCell ref="DJ5:DK5"/>
-    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="AF1:BI1"/>
+    <mergeCell ref="BJ1:BT1"/>
+    <mergeCell ref="BU1:BY1"/>
+    <mergeCell ref="BZ1:CG1"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="CB6:CC6"/>
+    <mergeCell ref="BK3:BN3"/>
+    <mergeCell ref="CN3:CP3"/>
+    <mergeCell ref="CQ3:CS3"/>
+    <mergeCell ref="BO4:BR4"/>
+    <mergeCell ref="BX4:BY4"/>
+    <mergeCell ref="BL5:BM5"/>
+    <mergeCell ref="BO5:BR5"/>
+    <mergeCell ref="BW5:BY5"/>
+    <mergeCell ref="CH5:CI5"/>
+    <mergeCell ref="CD5:CF5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="B6:H6"/>
     <mergeCell ref="I7:S7"/>
     <mergeCell ref="T7:AA7"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="T6:AE6"/>
+    <mergeCell ref="R6:S6"/>
     <mergeCell ref="AD7:AE7"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AK7:BI7"/>
-    <mergeCell ref="AF7:AG7"/>
-    <mergeCell ref="CH1:DI1"/>
-    <mergeCell ref="DJ1:DU1"/>
-    <mergeCell ref="DV1:EB1"/>
-    <mergeCell ref="DV7:EB7"/>
-    <mergeCell ref="AT5:AW5"/>
-    <mergeCell ref="AX5:BA5"/>
-    <mergeCell ref="BB5:BE5"/>
-    <mergeCell ref="BF5:BI5"/>
-    <mergeCell ref="BJ7:BT7"/>
-    <mergeCell ref="BU7:BY7"/>
-    <mergeCell ref="BZ7:CG7"/>
-    <mergeCell ref="CH7:DI7"/>
-    <mergeCell ref="DJ7:DU7"/>
-    <mergeCell ref="BZ6:CA6"/>
-    <mergeCell ref="BU6:BY6"/>
-    <mergeCell ref="BJ6:BR6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AD4" r:id="rId1" xr:uid="{F3767099-F5B4-4A43-9EF8-725310DD37E5}"/>
@@ -4153,16 +4156,22 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 OFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4426,20 +4435,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="83a87e31-bf32-46ab-8e70-9fa18461fa4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ede1785e-3bac-4a90-a48c-62cc0231644e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E6DF85-604C-4C11-B168-A00921BCEA51}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF050CE3-396B-4D35-A168-28F84B0244F1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4465,25 +4482,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF050CE3-396B-4D35-A168-28F84B0244F1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34E6DF85-604C-4C11-B168-A00921BCEA51}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="ede1785e-3bac-4a90-a48c-62cc0231644e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="83a87e31-bf32-46ab-8e70-9fa18461fa4d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="6c5f9a5a-0dad-4595-a39a-6416e9fb7054"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{bf346810-9c7d-43de-a872-24a2ef3995a8}" enabled="0" method="" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" removed="1"/>
+  <clbl:label id="{fbd41ebe-fca6-4f2c-aecb-bf3a17e72416}" enabled="1" method="Privileged" siteId="{bf346810-9c7d-43de-a872-24a2ef3995a8}" contentBits="3" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>